<commit_message>
Removed previous dataset results and added results for 5k elements.
</commit_message>
<xml_diff>
--- a/z_HybridAlgorithmResults.xlsx
+++ b/z_HybridAlgorithmResults.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="11">
   <si>
     <t>Bubble</t>
   </si>
@@ -35,55 +35,28 @@
     <t>Hybrid</t>
   </si>
   <si>
-    <t>Hybrid (2000 elements) in ms</t>
+    <t>Average Runtime per Number of Elements</t>
   </si>
   <si>
-    <t>Bubble (2000 elements) in ms</t>
+    <t>Hybrid Sorting Algorithm Runtime in ms</t>
   </si>
   <si>
-    <t>Merge (2000 elements) in ms</t>
+    <t>Bubble Sorting Algorithm Runtime in ms</t>
   </si>
   <si>
-    <t>Hybrid (4000 elements) in ms</t>
+    <t>Merge Sorting Algorithm Runtime in ms</t>
   </si>
   <si>
-    <t>Bubble (4000 elements) in ms</t>
+    <t>5,000 Elements</t>
   </si>
   <si>
-    <t>Merge (4000 elements) in ms</t>
+    <t>10,000 Elements</t>
   </si>
   <si>
-    <t>Hybrid (6000 elements) in ms</t>
+    <t>15,000 Elements</t>
   </si>
   <si>
-    <t>Bubble (6000 elements) in ms</t>
-  </si>
-  <si>
-    <t>Merge (6000 elements) in ms</t>
-  </si>
-  <si>
-    <t>Hybrid (8000 elements) in ms</t>
-  </si>
-  <si>
-    <t>Bubble (8000 elements) in ms</t>
-  </si>
-  <si>
-    <t>Merge (8000 elements) in ms</t>
-  </si>
-  <si>
-    <t>2000 Elements</t>
-  </si>
-  <si>
-    <t>4000 Elements</t>
-  </si>
-  <si>
-    <t>6000 Elements</t>
-  </si>
-  <si>
-    <t>8000 Elements</t>
-  </si>
-  <si>
-    <t>Average Runtime per Number of Elements</t>
+    <t>20,000 Elements</t>
   </si>
 </sst>
 </file>
@@ -322,7 +295,7 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="medium">
+      <top style="thin">
         <color indexed="64"/>
       </top>
       <bottom style="thin">
@@ -334,10 +307,10 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
         <color indexed="64"/>
       </top>
       <bottom style="thin">
@@ -346,51 +319,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
@@ -431,6 +359,45 @@
         <color indexed="64"/>
       </top>
       <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -439,7 +406,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -483,15 +450,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -507,6 +465,57 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -516,52 +525,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -846,8 +810,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:P29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I32" sqref="I32"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -859,175 +823,159 @@
     <row r="1" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="2"/>
-      <c r="C2" s="39" t="s">
-        <v>19</v>
-      </c>
-      <c r="D2" s="40"/>
-      <c r="E2" s="40"/>
-      <c r="F2" s="40"/>
-      <c r="G2" s="40"/>
-      <c r="H2" s="40"/>
-      <c r="I2" s="40"/>
-      <c r="J2" s="40"/>
-      <c r="K2" s="41"/>
+      <c r="C2" s="29" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="30"/>
+      <c r="E2" s="30"/>
+      <c r="F2" s="30"/>
+      <c r="G2" s="30"/>
+      <c r="H2" s="30"/>
+      <c r="I2" s="30"/>
+      <c r="J2" s="30"/>
+      <c r="K2" s="31"/>
     </row>
     <row r="3" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="3"/>
-      <c r="C3" s="15">
-        <v>2000</v>
-      </c>
-      <c r="D3" s="16">
-        <v>4000</v>
-      </c>
-      <c r="E3" s="16">
-        <v>6000</v>
-      </c>
-      <c r="F3" s="16">
-        <v>8000</v>
-      </c>
-      <c r="G3" s="16">
+      <c r="C3" s="36">
+        <v>5000</v>
+      </c>
+      <c r="D3" s="35">
         <v>10000</v>
       </c>
-      <c r="H3" s="16">
-        <v>12000</v>
-      </c>
-      <c r="I3" s="16">
-        <v>14000</v>
-      </c>
-      <c r="J3" s="16">
-        <v>16000</v>
-      </c>
-      <c r="K3" s="17">
-        <v>18000</v>
+      <c r="E3" s="35">
+        <v>15000</v>
+      </c>
+      <c r="F3" s="35">
+        <v>20000</v>
+      </c>
+      <c r="G3" s="35">
+        <v>25000</v>
+      </c>
+      <c r="H3" s="35">
+        <v>30000</v>
+      </c>
+      <c r="I3" s="35">
+        <v>35000</v>
+      </c>
+      <c r="J3" s="35">
+        <v>40000</v>
+      </c>
+      <c r="K3" s="40">
+        <v>45000</v>
       </c>
     </row>
     <row r="4" spans="2:16" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="C4" s="18">
-        <v>6.4048199999999991</v>
-      </c>
-      <c r="D4" s="19">
-        <v>24.922080000000001</v>
-      </c>
-      <c r="E4" s="19">
-        <v>55.545540000000003</v>
-      </c>
-      <c r="F4" s="19"/>
-      <c r="G4" s="19"/>
-      <c r="H4" s="19"/>
-      <c r="I4" s="19"/>
-      <c r="J4" s="19"/>
-      <c r="K4" s="20"/>
+        <v>2</v>
+      </c>
+      <c r="C4" s="37">
+        <v>2.6657999999999999</v>
+      </c>
+      <c r="D4" s="38"/>
+      <c r="E4" s="38"/>
+      <c r="F4" s="38"/>
+      <c r="G4" s="38"/>
+      <c r="H4" s="38"/>
+      <c r="I4" s="38"/>
+      <c r="J4" s="38"/>
+      <c r="K4" s="39"/>
     </row>
     <row r="5" spans="2:16" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="13" t="s">
-        <v>1</v>
-      </c>
-      <c r="C5" s="21">
-        <v>2.0217599999999996</v>
-      </c>
-      <c r="D5" s="11">
-        <v>3.7152400000000001</v>
-      </c>
-      <c r="E5" s="11">
-        <v>5.4830799999999993</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="C5" s="15">
+        <v>37.69726</v>
+      </c>
+      <c r="D5" s="11"/>
+      <c r="E5" s="11"/>
       <c r="F5" s="11"/>
       <c r="G5" s="11"/>
       <c r="H5" s="11"/>
       <c r="I5" s="11"/>
       <c r="J5" s="11"/>
-      <c r="K5" s="22"/>
+      <c r="K5" s="16"/>
     </row>
     <row r="6" spans="2:16" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="C6" s="23">
-        <v>1.1597200000000001</v>
-      </c>
-      <c r="D6" s="24">
-        <v>2.0771000000000002</v>
-      </c>
-      <c r="E6" s="24">
-        <v>3.1892399999999999</v>
-      </c>
-      <c r="F6" s="24"/>
-      <c r="G6" s="24"/>
-      <c r="H6" s="24"/>
-      <c r="I6" s="24"/>
-      <c r="J6" s="24"/>
-      <c r="K6" s="25"/>
+        <v>1</v>
+      </c>
+      <c r="C6" s="17">
+        <v>7.6337600000000005</v>
+      </c>
+      <c r="D6" s="18"/>
+      <c r="E6" s="18"/>
+      <c r="F6" s="18"/>
+      <c r="G6" s="18"/>
+      <c r="H6" s="18"/>
+      <c r="I6" s="18"/>
+      <c r="J6" s="18"/>
+      <c r="K6" s="19"/>
     </row>
     <row r="7" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="8" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B8" s="30" t="s">
-        <v>15</v>
-      </c>
-      <c r="C8" s="31"/>
-      <c r="D8" s="32"/>
-      <c r="F8" s="30" t="s">
-        <v>16</v>
-      </c>
-      <c r="G8" s="31"/>
-      <c r="H8" s="32"/>
-      <c r="J8" s="30" t="s">
-        <v>17</v>
-      </c>
-      <c r="K8" s="31"/>
-      <c r="L8" s="32"/>
-      <c r="N8" s="30" t="s">
-        <v>18</v>
-      </c>
-      <c r="O8" s="31"/>
-      <c r="P8" s="32"/>
+      <c r="B8" s="29" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="30"/>
+      <c r="D8" s="31"/>
+      <c r="F8" s="29" t="s">
+        <v>8</v>
+      </c>
+      <c r="G8" s="30"/>
+      <c r="H8" s="31"/>
+      <c r="J8" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="K8" s="30"/>
+      <c r="L8" s="31"/>
+      <c r="N8" s="29" t="s">
+        <v>10</v>
+      </c>
+      <c r="O8" s="30"/>
+      <c r="P8" s="31"/>
     </row>
     <row r="9" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="33"/>
-      <c r="C9" s="34"/>
-      <c r="D9" s="35"/>
-      <c r="F9" s="33"/>
-      <c r="G9" s="34"/>
-      <c r="H9" s="35"/>
-      <c r="J9" s="33"/>
-      <c r="K9" s="34"/>
-      <c r="L9" s="35"/>
-      <c r="N9" s="33"/>
-      <c r="O9" s="34"/>
-      <c r="P9" s="35"/>
-    </row>
-    <row r="10" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B10" s="36" t="s">
-        <v>3</v>
+      <c r="B9" s="32"/>
+      <c r="C9" s="33"/>
+      <c r="D9" s="34"/>
+      <c r="F9" s="32"/>
+      <c r="G9" s="33"/>
+      <c r="H9" s="34"/>
+      <c r="J9" s="32"/>
+      <c r="K9" s="33"/>
+      <c r="L9" s="34"/>
+      <c r="N9" s="32"/>
+      <c r="O9" s="33"/>
+      <c r="P9" s="34"/>
+    </row>
+    <row r="10" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="26" t="s">
+        <v>4</v>
       </c>
       <c r="C10" s="4">
         <v>1</v>
       </c>
       <c r="D10" s="5">
-        <v>1.1128</v>
-      </c>
-      <c r="F10" s="36" t="s">
-        <v>6</v>
+        <v>2.6745999999999999</v>
+      </c>
+      <c r="F10" s="26" t="s">
+        <v>4</v>
       </c>
       <c r="G10" s="4">
         <v>1</v>
       </c>
-      <c r="H10" s="5">
-        <v>1.9626999999999999</v>
-      </c>
-      <c r="J10" s="36" t="s">
-        <v>9</v>
+      <c r="H10" s="5"/>
+      <c r="J10" s="26" t="s">
+        <v>4</v>
       </c>
       <c r="K10" s="4">
         <v>1</v>
       </c>
-      <c r="L10" s="5">
-        <v>3.2054999999999998</v>
-      </c>
-      <c r="N10" s="36" t="s">
-        <v>12</v>
+      <c r="L10" s="5"/>
+      <c r="N10" s="26" t="s">
+        <v>4</v>
       </c>
       <c r="O10" s="4">
         <v>1</v>
@@ -1035,112 +983,96 @@
       <c r="P10" s="5"/>
     </row>
     <row r="11" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B11" s="37"/>
+      <c r="B11" s="27"/>
       <c r="C11" s="6">
         <v>2</v>
       </c>
       <c r="D11" s="7">
-        <v>1.1745000000000001</v>
-      </c>
-      <c r="F11" s="37"/>
+        <v>2.6539999999999999</v>
+      </c>
+      <c r="F11" s="27"/>
       <c r="G11" s="6">
         <v>2</v>
       </c>
-      <c r="H11" s="7">
-        <v>2.625</v>
-      </c>
-      <c r="J11" s="37"/>
+      <c r="H11" s="7"/>
+      <c r="J11" s="27"/>
       <c r="K11" s="6">
         <v>2</v>
       </c>
-      <c r="L11" s="7">
-        <v>3.1863000000000001</v>
-      </c>
-      <c r="N11" s="37"/>
+      <c r="L11" s="7"/>
+      <c r="N11" s="27"/>
       <c r="O11" s="6">
         <v>2</v>
       </c>
       <c r="P11" s="7"/>
     </row>
     <row r="12" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B12" s="37"/>
+      <c r="B12" s="27"/>
       <c r="C12" s="6">
         <v>3</v>
       </c>
       <c r="D12" s="7">
-        <v>1.0495000000000001</v>
-      </c>
-      <c r="F12" s="37"/>
+        <v>2.6448</v>
+      </c>
+      <c r="F12" s="27"/>
       <c r="G12" s="6">
         <v>3</v>
       </c>
-      <c r="H12" s="7">
-        <v>2.04</v>
-      </c>
-      <c r="J12" s="37"/>
+      <c r="H12" s="7"/>
+      <c r="J12" s="27"/>
       <c r="K12" s="6">
         <v>3</v>
       </c>
-      <c r="L12" s="7">
-        <v>3.2174999999999998</v>
-      </c>
-      <c r="N12" s="37"/>
+      <c r="L12" s="7"/>
+      <c r="N12" s="27"/>
       <c r="O12" s="6">
         <v>3</v>
       </c>
       <c r="P12" s="7"/>
     </row>
     <row r="13" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B13" s="37"/>
+      <c r="B13" s="27"/>
       <c r="C13" s="6">
         <v>4</v>
       </c>
       <c r="D13" s="7">
-        <v>1.18</v>
-      </c>
-      <c r="F13" s="37"/>
+        <v>2.6669999999999998</v>
+      </c>
+      <c r="F13" s="27"/>
       <c r="G13" s="6">
         <v>4</v>
       </c>
-      <c r="H13" s="7">
-        <v>1.8332999999999999</v>
-      </c>
-      <c r="J13" s="37"/>
+      <c r="H13" s="7"/>
+      <c r="J13" s="27"/>
       <c r="K13" s="6">
         <v>4</v>
       </c>
-      <c r="L13" s="7">
-        <v>3.2040000000000002</v>
-      </c>
-      <c r="N13" s="37"/>
+      <c r="L13" s="7"/>
+      <c r="N13" s="27"/>
       <c r="O13" s="6">
         <v>4</v>
       </c>
       <c r="P13" s="7"/>
     </row>
     <row r="14" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="38"/>
+      <c r="B14" s="28"/>
       <c r="C14" s="8">
         <v>5</v>
       </c>
       <c r="D14" s="9">
-        <v>1.2818000000000001</v>
-      </c>
-      <c r="F14" s="38"/>
+        <v>2.6886000000000001</v>
+      </c>
+      <c r="F14" s="28"/>
       <c r="G14" s="8">
         <v>5</v>
       </c>
-      <c r="H14" s="9">
-        <v>1.9245000000000001</v>
-      </c>
-      <c r="J14" s="38"/>
+      <c r="H14" s="9"/>
+      <c r="J14" s="28"/>
       <c r="K14" s="8">
         <v>5</v>
       </c>
-      <c r="L14" s="9">
-        <v>3.1328999999999998</v>
-      </c>
-      <c r="N14" s="38"/>
+      <c r="L14" s="9"/>
+      <c r="N14" s="28"/>
       <c r="O14" s="8">
         <v>5</v>
       </c>
@@ -1148,25 +1080,25 @@
     </row>
     <row r="15" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B15" s="3"/>
-      <c r="C15" s="27"/>
+      <c r="C15" s="21"/>
       <c r="D15" s="10">
         <f>AVERAGE(D10:D14)</f>
-        <v>1.1597200000000001</v>
+        <v>2.6657999999999999</v>
       </c>
       <c r="F15" s="3"/>
-      <c r="G15" s="27"/>
-      <c r="H15" s="10">
+      <c r="G15" s="21"/>
+      <c r="H15" s="10" t="e">
         <f>AVERAGE(H10:H14)</f>
-        <v>2.0771000000000002</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="J15" s="3"/>
-      <c r="K15" s="27"/>
-      <c r="L15" s="10">
+      <c r="K15" s="21"/>
+      <c r="L15" s="10" t="e">
         <f>AVERAGE(L10:L14)</f>
-        <v>3.1892399999999999</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="N15" s="3"/>
-      <c r="O15" s="27"/>
+      <c r="O15" s="21"/>
       <c r="P15" s="10" t="e">
         <f>AVERAGE(P10:P14)</f>
         <v>#DIV/0!</v>
@@ -1174,48 +1106,44 @@
     </row>
     <row r="16" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B16" s="3"/>
-      <c r="C16" s="27"/>
-      <c r="D16" s="26"/>
+      <c r="C16" s="21"/>
+      <c r="D16" s="20"/>
       <c r="F16" s="3"/>
-      <c r="G16" s="27"/>
-      <c r="H16" s="26"/>
+      <c r="G16" s="21"/>
+      <c r="H16" s="20"/>
       <c r="J16" s="3"/>
-      <c r="K16" s="27"/>
-      <c r="L16" s="26"/>
+      <c r="K16" s="21"/>
+      <c r="L16" s="20"/>
       <c r="N16" s="3"/>
-      <c r="O16" s="27"/>
-      <c r="P16" s="26"/>
-    </row>
-    <row r="17" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B17" s="36" t="s">
-        <v>4</v>
+      <c r="O16" s="21"/>
+      <c r="P16" s="20"/>
+    </row>
+    <row r="17" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="26" t="s">
+        <v>5</v>
       </c>
       <c r="C17" s="4">
         <v>1</v>
       </c>
       <c r="D17" s="5">
-        <v>6.3722000000000003</v>
-      </c>
-      <c r="F17" s="36" t="s">
-        <v>7</v>
+        <v>37.5824</v>
+      </c>
+      <c r="F17" s="26" t="s">
+        <v>5</v>
       </c>
       <c r="G17" s="4">
         <v>1</v>
       </c>
-      <c r="H17" s="5">
-        <v>24.009399999999999</v>
-      </c>
-      <c r="J17" s="36" t="s">
-        <v>10</v>
+      <c r="H17" s="5"/>
+      <c r="J17" s="26" t="s">
+        <v>5</v>
       </c>
       <c r="K17" s="4">
         <v>1</v>
       </c>
-      <c r="L17" s="5">
-        <v>55.846400000000003</v>
-      </c>
-      <c r="N17" s="36" t="s">
-        <v>13</v>
+      <c r="L17" s="5"/>
+      <c r="N17" s="26" t="s">
+        <v>5</v>
       </c>
       <c r="O17" s="4">
         <v>1</v>
@@ -1223,112 +1151,96 @@
       <c r="P17" s="5"/>
     </row>
     <row r="18" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B18" s="37"/>
+      <c r="B18" s="27"/>
       <c r="C18" s="6">
         <v>2</v>
       </c>
       <c r="D18" s="7">
-        <v>6.2575000000000003</v>
-      </c>
-      <c r="F18" s="37"/>
+        <v>37.5227</v>
+      </c>
+      <c r="F18" s="27"/>
       <c r="G18" s="6">
         <v>2</v>
       </c>
-      <c r="H18" s="7">
-        <v>23.9634</v>
-      </c>
-      <c r="J18" s="37"/>
+      <c r="H18" s="7"/>
+      <c r="J18" s="27"/>
       <c r="K18" s="6">
         <v>2</v>
       </c>
-      <c r="L18" s="7">
-        <v>54.672600000000003</v>
-      </c>
-      <c r="N18" s="37"/>
+      <c r="L18" s="7"/>
+      <c r="N18" s="27"/>
       <c r="O18" s="6">
         <v>2</v>
       </c>
       <c r="P18" s="7"/>
     </row>
     <row r="19" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B19" s="37"/>
+      <c r="B19" s="27"/>
       <c r="C19" s="6">
         <v>3</v>
       </c>
       <c r="D19" s="7">
-        <v>6.3083</v>
-      </c>
-      <c r="F19" s="37"/>
+        <v>37.150199999999998</v>
+      </c>
+      <c r="F19" s="27"/>
       <c r="G19" s="6">
         <v>3</v>
       </c>
-      <c r="H19" s="7">
-        <v>24.928100000000001</v>
-      </c>
-      <c r="J19" s="37"/>
+      <c r="H19" s="7"/>
+      <c r="J19" s="27"/>
       <c r="K19" s="6">
         <v>3</v>
       </c>
-      <c r="L19" s="7">
-        <v>54.997700000000002</v>
-      </c>
-      <c r="N19" s="37"/>
+      <c r="L19" s="7"/>
+      <c r="N19" s="27"/>
       <c r="O19" s="6">
         <v>3</v>
       </c>
       <c r="P19" s="7"/>
     </row>
     <row r="20" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B20" s="37"/>
+      <c r="B20" s="27"/>
       <c r="C20" s="6">
         <v>4</v>
       </c>
       <c r="D20" s="7">
-        <v>6.9898999999999996</v>
-      </c>
-      <c r="F20" s="37"/>
+        <v>37.191299999999998</v>
+      </c>
+      <c r="F20" s="27"/>
       <c r="G20" s="6">
         <v>4</v>
       </c>
-      <c r="H20" s="7">
-        <v>26.6373</v>
-      </c>
-      <c r="J20" s="37"/>
+      <c r="H20" s="7"/>
+      <c r="J20" s="27"/>
       <c r="K20" s="6">
         <v>4</v>
       </c>
-      <c r="L20" s="7">
-        <v>55.184199999999997</v>
-      </c>
-      <c r="N20" s="37"/>
+      <c r="L20" s="7"/>
+      <c r="N20" s="27"/>
       <c r="O20" s="6">
         <v>4</v>
       </c>
       <c r="P20" s="7"/>
     </row>
     <row r="21" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="38"/>
+      <c r="B21" s="28"/>
       <c r="C21" s="8">
         <v>5</v>
       </c>
       <c r="D21" s="9">
-        <v>6.0961999999999996</v>
-      </c>
-      <c r="F21" s="38"/>
+        <v>39.039700000000003</v>
+      </c>
+      <c r="F21" s="28"/>
       <c r="G21" s="8">
         <v>5</v>
       </c>
-      <c r="H21" s="9">
-        <v>25.072199999999999</v>
-      </c>
-      <c r="J21" s="38"/>
+      <c r="H21" s="9"/>
+      <c r="J21" s="28"/>
       <c r="K21" s="8">
         <v>5</v>
       </c>
-      <c r="L21" s="9">
-        <v>57.026800000000001</v>
-      </c>
-      <c r="N21" s="38"/>
+      <c r="L21" s="9"/>
+      <c r="N21" s="28"/>
       <c r="O21" s="8">
         <v>5</v>
       </c>
@@ -1336,25 +1248,25 @@
     </row>
     <row r="22" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B22" s="3"/>
-      <c r="C22" s="27"/>
+      <c r="C22" s="21"/>
       <c r="D22" s="10">
         <f>AVERAGE(D17:D21)</f>
-        <v>6.4048199999999991</v>
+        <v>37.69726</v>
       </c>
       <c r="F22" s="3"/>
-      <c r="G22" s="27"/>
-      <c r="H22" s="10">
+      <c r="G22" s="21"/>
+      <c r="H22" s="10" t="e">
         <f>AVERAGE(H17:H21)</f>
-        <v>24.922080000000001</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="J22" s="3"/>
-      <c r="K22" s="27"/>
-      <c r="L22" s="10">
+      <c r="K22" s="21"/>
+      <c r="L22" s="10" t="e">
         <f>AVERAGE(L17:L21)</f>
-        <v>55.545540000000003</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="N22" s="3"/>
-      <c r="O22" s="27"/>
+      <c r="O22" s="21"/>
       <c r="P22" s="10" t="e">
         <f>AVERAGE(P17:P21)</f>
         <v>#DIV/0!</v>
@@ -1362,48 +1274,44 @@
     </row>
     <row r="23" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B23" s="3"/>
-      <c r="C23" s="27"/>
-      <c r="D23" s="26"/>
+      <c r="C23" s="21"/>
+      <c r="D23" s="20"/>
       <c r="F23" s="3"/>
-      <c r="G23" s="27"/>
-      <c r="H23" s="26"/>
+      <c r="G23" s="21"/>
+      <c r="H23" s="20"/>
       <c r="J23" s="3"/>
-      <c r="K23" s="27"/>
-      <c r="L23" s="26"/>
+      <c r="K23" s="21"/>
+      <c r="L23" s="20"/>
       <c r="N23" s="3"/>
-      <c r="O23" s="27"/>
-      <c r="P23" s="26"/>
-    </row>
-    <row r="24" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B24" s="36" t="s">
-        <v>5</v>
+      <c r="O23" s="21"/>
+      <c r="P23" s="20"/>
+    </row>
+    <row r="24" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B24" s="26" t="s">
+        <v>6</v>
       </c>
       <c r="C24" s="4">
         <v>1</v>
       </c>
       <c r="D24" s="5">
-        <v>2.1343999999999999</v>
-      </c>
-      <c r="F24" s="36" t="s">
-        <v>8</v>
+        <v>8.2642000000000007</v>
+      </c>
+      <c r="F24" s="26" t="s">
+        <v>6</v>
       </c>
       <c r="G24" s="4">
         <v>1</v>
       </c>
-      <c r="H24" s="5">
-        <v>3.5375999999999999</v>
-      </c>
-      <c r="J24" s="36" t="s">
-        <v>11</v>
+      <c r="H24" s="5"/>
+      <c r="J24" s="26" t="s">
+        <v>6</v>
       </c>
       <c r="K24" s="4">
         <v>1</v>
       </c>
-      <c r="L24" s="5">
-        <v>5.4630000000000001</v>
-      </c>
-      <c r="N24" s="36" t="s">
-        <v>14</v>
+      <c r="L24" s="5"/>
+      <c r="N24" s="26" t="s">
+        <v>6</v>
       </c>
       <c r="O24" s="4">
         <v>1</v>
@@ -1411,138 +1319,122 @@
       <c r="P24" s="5"/>
     </row>
     <row r="25" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B25" s="37"/>
+      <c r="B25" s="27"/>
       <c r="C25" s="6">
         <v>2</v>
       </c>
       <c r="D25" s="7">
-        <v>2.0802999999999998</v>
-      </c>
-      <c r="F25" s="37"/>
+        <v>7.4324000000000003</v>
+      </c>
+      <c r="F25" s="27"/>
       <c r="G25" s="6">
         <v>2</v>
       </c>
-      <c r="H25" s="7">
-        <v>3.6453000000000002</v>
-      </c>
-      <c r="J25" s="37"/>
+      <c r="H25" s="7"/>
+      <c r="J25" s="27"/>
       <c r="K25" s="6">
         <v>2</v>
       </c>
-      <c r="L25" s="7">
-        <v>5.4660000000000002</v>
-      </c>
-      <c r="N25" s="37"/>
+      <c r="L25" s="7"/>
+      <c r="N25" s="27"/>
       <c r="O25" s="6">
         <v>2</v>
       </c>
       <c r="P25" s="7"/>
     </row>
     <row r="26" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B26" s="37"/>
+      <c r="B26" s="27"/>
       <c r="C26" s="6">
         <v>3</v>
       </c>
       <c r="D26" s="7">
-        <v>1.9058999999999999</v>
-      </c>
-      <c r="F26" s="37"/>
+        <v>7.1902999999999997</v>
+      </c>
+      <c r="F26" s="27"/>
       <c r="G26" s="6">
         <v>3</v>
       </c>
-      <c r="H26" s="26">
-        <v>3.72</v>
-      </c>
-      <c r="J26" s="37"/>
+      <c r="H26" s="7"/>
+      <c r="J26" s="27"/>
       <c r="K26" s="6">
         <v>3</v>
       </c>
-      <c r="L26" s="7">
-        <v>5.6996000000000002</v>
-      </c>
-      <c r="N26" s="37"/>
+      <c r="L26" s="7"/>
+      <c r="N26" s="27"/>
       <c r="O26" s="6">
         <v>3</v>
       </c>
-      <c r="P26" s="26"/>
+      <c r="P26" s="7"/>
     </row>
     <row r="27" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B27" s="37"/>
+      <c r="B27" s="27"/>
       <c r="C27" s="6">
         <v>4</v>
       </c>
       <c r="D27" s="7">
-        <v>2.0171000000000001</v>
-      </c>
-      <c r="F27" s="37"/>
+        <v>7.7202000000000002</v>
+      </c>
+      <c r="F27" s="27"/>
       <c r="G27" s="6">
         <v>4</v>
       </c>
-      <c r="H27" s="26">
-        <v>3.7803</v>
-      </c>
-      <c r="J27" s="37"/>
+      <c r="H27" s="7"/>
+      <c r="J27" s="27"/>
       <c r="K27" s="6">
         <v>4</v>
       </c>
-      <c r="L27" s="7">
-        <v>5.3846999999999996</v>
-      </c>
-      <c r="N27" s="37"/>
+      <c r="L27" s="7"/>
+      <c r="N27" s="27"/>
       <c r="O27" s="6">
         <v>4</v>
       </c>
-      <c r="P27" s="26"/>
+      <c r="P27" s="7"/>
     </row>
     <row r="28" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="38"/>
+      <c r="B28" s="28"/>
       <c r="C28" s="8">
         <v>5</v>
       </c>
       <c r="D28" s="9">
-        <v>1.9711000000000001</v>
-      </c>
-      <c r="F28" s="38"/>
+        <v>7.5617000000000001</v>
+      </c>
+      <c r="F28" s="28"/>
       <c r="G28" s="8">
         <v>5</v>
       </c>
-      <c r="H28" s="9">
-        <v>3.8929999999999998</v>
-      </c>
-      <c r="J28" s="38"/>
+      <c r="H28" s="9"/>
+      <c r="J28" s="28"/>
       <c r="K28" s="8">
         <v>5</v>
       </c>
-      <c r="L28" s="9">
-        <v>5.4020999999999999</v>
-      </c>
-      <c r="N28" s="38"/>
+      <c r="L28" s="9"/>
+      <c r="N28" s="28"/>
       <c r="O28" s="8">
         <v>5</v>
       </c>
       <c r="P28" s="9"/>
     </row>
     <row r="29" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="28"/>
-      <c r="C29" s="29"/>
+      <c r="B29" s="22"/>
+      <c r="C29" s="23"/>
       <c r="D29" s="10">
         <f>AVERAGE(D24:D28)</f>
-        <v>2.0217599999999996</v>
-      </c>
-      <c r="F29" s="28"/>
-      <c r="G29" s="29"/>
-      <c r="H29" s="10">
+        <v>7.6337600000000005</v>
+      </c>
+      <c r="F29" s="24"/>
+      <c r="G29" s="25"/>
+      <c r="H29" s="10" t="e">
         <f>AVERAGE(H24:H28)</f>
-        <v>3.7152400000000001</v>
-      </c>
-      <c r="J29" s="28"/>
-      <c r="K29" s="29"/>
-      <c r="L29" s="10">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J29" s="24"/>
+      <c r="K29" s="25"/>
+      <c r="L29" s="10" t="e">
         <f>AVERAGE(L24:L28)</f>
-        <v>5.4830799999999993</v>
-      </c>
-      <c r="N29" s="28"/>
-      <c r="O29" s="29"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N29" s="24"/>
+      <c r="O29" s="25"/>
       <c r="P29" s="10" t="e">
         <f>AVERAGE(P24:P28)</f>
         <v>#DIV/0!</v>
@@ -1550,6 +1442,12 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="N8:P9"/>
+    <mergeCell ref="N10:N14"/>
+    <mergeCell ref="J17:J21"/>
+    <mergeCell ref="N17:N21"/>
+    <mergeCell ref="J24:J28"/>
+    <mergeCell ref="N24:N28"/>
     <mergeCell ref="C2:K2"/>
     <mergeCell ref="B10:B14"/>
     <mergeCell ref="B17:B21"/>
@@ -1561,12 +1459,6 @@
     <mergeCell ref="B8:D9"/>
     <mergeCell ref="F8:H9"/>
     <mergeCell ref="J8:L9"/>
-    <mergeCell ref="N8:P9"/>
-    <mergeCell ref="N10:N14"/>
-    <mergeCell ref="J17:J21"/>
-    <mergeCell ref="N17:N21"/>
-    <mergeCell ref="J24:J28"/>
-    <mergeCell ref="N24:N28"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Renamed the 5000 Elements Folder
</commit_message>
<xml_diff>
--- a/z_HybridAlgorithmResults.xlsx
+++ b/z_HybridAlgorithmResults.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="12">
   <si>
     <t>Bubble</t>
   </si>
@@ -33,9 +33,6 @@
   </si>
   <si>
     <t>Hybrid</t>
-  </si>
-  <si>
-    <t>Average Runtime per Number of Elements</t>
   </si>
   <si>
     <t>Hybrid Sorting Algorithm Runtime in ms</t>
@@ -57,6 +54,12 @@
   </si>
   <si>
     <t>20,000 Elements</t>
+  </si>
+  <si>
+    <t>Average Runtime per Number of Elements in ms</t>
+  </si>
+  <si>
+    <t>Number of Elements (n)</t>
   </si>
 </sst>
 </file>
@@ -406,7 +409,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -483,6 +486,42 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -492,40 +531,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -810,8 +816,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:P29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17:F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -823,45 +829,47 @@
     <row r="1" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="2"/>
-      <c r="C2" s="29" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2" s="30"/>
-      <c r="E2" s="30"/>
-      <c r="F2" s="30"/>
-      <c r="G2" s="30"/>
-      <c r="H2" s="30"/>
-      <c r="I2" s="30"/>
-      <c r="J2" s="30"/>
-      <c r="K2" s="31"/>
-    </row>
-    <row r="3" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="3"/>
-      <c r="C3" s="36">
+      <c r="C2" s="32" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="33"/>
+      <c r="E2" s="33"/>
+      <c r="F2" s="33"/>
+      <c r="G2" s="33"/>
+      <c r="H2" s="33"/>
+      <c r="I2" s="33"/>
+      <c r="J2" s="33"/>
+      <c r="K2" s="34"/>
+    </row>
+    <row r="3" spans="2:16" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="41" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="27">
         <v>5000</v>
       </c>
-      <c r="D3" s="35">
+      <c r="D3" s="26">
         <v>10000</v>
       </c>
-      <c r="E3" s="35">
+      <c r="E3" s="26">
         <v>15000</v>
       </c>
-      <c r="F3" s="35">
+      <c r="F3" s="26">
         <v>20000</v>
       </c>
-      <c r="G3" s="35">
+      <c r="G3" s="26">
         <v>25000</v>
       </c>
-      <c r="H3" s="35">
+      <c r="H3" s="26">
         <v>30000</v>
       </c>
-      <c r="I3" s="35">
+      <c r="I3" s="26">
         <v>35000</v>
       </c>
-      <c r="J3" s="35">
+      <c r="J3" s="26">
         <v>40000</v>
       </c>
-      <c r="K3" s="40">
+      <c r="K3" s="31">
         <v>45000</v>
       </c>
     </row>
@@ -869,17 +877,17 @@
       <c r="B4" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="37">
+      <c r="C4" s="28">
         <v>2.6657999999999999</v>
       </c>
-      <c r="D4" s="38"/>
-      <c r="E4" s="38"/>
-      <c r="F4" s="38"/>
-      <c r="G4" s="38"/>
-      <c r="H4" s="38"/>
-      <c r="I4" s="38"/>
-      <c r="J4" s="38"/>
-      <c r="K4" s="39"/>
+      <c r="D4" s="29"/>
+      <c r="E4" s="29"/>
+      <c r="F4" s="29"/>
+      <c r="G4" s="29"/>
+      <c r="H4" s="29"/>
+      <c r="I4" s="29"/>
+      <c r="J4" s="29"/>
+      <c r="K4" s="30"/>
     </row>
     <row r="5" spans="2:16" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="13" t="s">
@@ -915,44 +923,44 @@
     </row>
     <row r="7" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="8" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B8" s="29" t="s">
+      <c r="B8" s="32" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="33"/>
+      <c r="D8" s="34"/>
+      <c r="F8" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="30"/>
-      <c r="D8" s="31"/>
-      <c r="F8" s="29" t="s">
+      <c r="G8" s="33"/>
+      <c r="H8" s="34"/>
+      <c r="J8" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="G8" s="30"/>
-      <c r="H8" s="31"/>
-      <c r="J8" s="29" t="s">
+      <c r="K8" s="33"/>
+      <c r="L8" s="34"/>
+      <c r="N8" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="K8" s="30"/>
-      <c r="L8" s="31"/>
-      <c r="N8" s="29" t="s">
-        <v>10</v>
-      </c>
-      <c r="O8" s="30"/>
-      <c r="P8" s="31"/>
+      <c r="O8" s="33"/>
+      <c r="P8" s="34"/>
     </row>
     <row r="9" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="32"/>
-      <c r="C9" s="33"/>
-      <c r="D9" s="34"/>
-      <c r="F9" s="32"/>
-      <c r="G9" s="33"/>
-      <c r="H9" s="34"/>
-      <c r="J9" s="32"/>
-      <c r="K9" s="33"/>
-      <c r="L9" s="34"/>
-      <c r="N9" s="32"/>
-      <c r="O9" s="33"/>
-      <c r="P9" s="34"/>
+      <c r="B9" s="35"/>
+      <c r="C9" s="36"/>
+      <c r="D9" s="37"/>
+      <c r="F9" s="35"/>
+      <c r="G9" s="36"/>
+      <c r="H9" s="37"/>
+      <c r="J9" s="35"/>
+      <c r="K9" s="36"/>
+      <c r="L9" s="37"/>
+      <c r="N9" s="35"/>
+      <c r="O9" s="36"/>
+      <c r="P9" s="37"/>
     </row>
     <row r="10" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="26" t="s">
-        <v>4</v>
+      <c r="B10" s="38" t="s">
+        <v>3</v>
       </c>
       <c r="C10" s="4">
         <v>1</v>
@@ -960,22 +968,22 @@
       <c r="D10" s="5">
         <v>2.6745999999999999</v>
       </c>
-      <c r="F10" s="26" t="s">
-        <v>4</v>
+      <c r="F10" s="38" t="s">
+        <v>3</v>
       </c>
       <c r="G10" s="4">
         <v>1</v>
       </c>
       <c r="H10" s="5"/>
-      <c r="J10" s="26" t="s">
-        <v>4</v>
+      <c r="J10" s="38" t="s">
+        <v>3</v>
       </c>
       <c r="K10" s="4">
         <v>1</v>
       </c>
       <c r="L10" s="5"/>
-      <c r="N10" s="26" t="s">
-        <v>4</v>
+      <c r="N10" s="38" t="s">
+        <v>3</v>
       </c>
       <c r="O10" s="4">
         <v>1</v>
@@ -983,96 +991,96 @@
       <c r="P10" s="5"/>
     </row>
     <row r="11" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B11" s="27"/>
+      <c r="B11" s="39"/>
       <c r="C11" s="6">
         <v>2</v>
       </c>
       <c r="D11" s="7">
         <v>2.6539999999999999</v>
       </c>
-      <c r="F11" s="27"/>
+      <c r="F11" s="39"/>
       <c r="G11" s="6">
         <v>2</v>
       </c>
       <c r="H11" s="7"/>
-      <c r="J11" s="27"/>
+      <c r="J11" s="39"/>
       <c r="K11" s="6">
         <v>2</v>
       </c>
       <c r="L11" s="7"/>
-      <c r="N11" s="27"/>
+      <c r="N11" s="39"/>
       <c r="O11" s="6">
         <v>2</v>
       </c>
       <c r="P11" s="7"/>
     </row>
     <row r="12" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B12" s="27"/>
+      <c r="B12" s="39"/>
       <c r="C12" s="6">
         <v>3</v>
       </c>
       <c r="D12" s="7">
         <v>2.6448</v>
       </c>
-      <c r="F12" s="27"/>
+      <c r="F12" s="39"/>
       <c r="G12" s="6">
         <v>3</v>
       </c>
       <c r="H12" s="7"/>
-      <c r="J12" s="27"/>
+      <c r="J12" s="39"/>
       <c r="K12" s="6">
         <v>3</v>
       </c>
       <c r="L12" s="7"/>
-      <c r="N12" s="27"/>
+      <c r="N12" s="39"/>
       <c r="O12" s="6">
         <v>3</v>
       </c>
       <c r="P12" s="7"/>
     </row>
     <row r="13" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B13" s="27"/>
+      <c r="B13" s="39"/>
       <c r="C13" s="6">
         <v>4</v>
       </c>
       <c r="D13" s="7">
         <v>2.6669999999999998</v>
       </c>
-      <c r="F13" s="27"/>
+      <c r="F13" s="39"/>
       <c r="G13" s="6">
         <v>4</v>
       </c>
       <c r="H13" s="7"/>
-      <c r="J13" s="27"/>
+      <c r="J13" s="39"/>
       <c r="K13" s="6">
         <v>4</v>
       </c>
       <c r="L13" s="7"/>
-      <c r="N13" s="27"/>
+      <c r="N13" s="39"/>
       <c r="O13" s="6">
         <v>4</v>
       </c>
       <c r="P13" s="7"/>
     </row>
     <row r="14" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="28"/>
+      <c r="B14" s="40"/>
       <c r="C14" s="8">
         <v>5</v>
       </c>
       <c r="D14" s="9">
         <v>2.6886000000000001</v>
       </c>
-      <c r="F14" s="28"/>
+      <c r="F14" s="40"/>
       <c r="G14" s="8">
         <v>5</v>
       </c>
       <c r="H14" s="9"/>
-      <c r="J14" s="28"/>
+      <c r="J14" s="40"/>
       <c r="K14" s="8">
         <v>5</v>
       </c>
       <c r="L14" s="9"/>
-      <c r="N14" s="28"/>
+      <c r="N14" s="40"/>
       <c r="O14" s="8">
         <v>5</v>
       </c>
@@ -1119,8 +1127,8 @@
       <c r="P16" s="20"/>
     </row>
     <row r="17" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="26" t="s">
-        <v>5</v>
+      <c r="B17" s="38" t="s">
+        <v>4</v>
       </c>
       <c r="C17" s="4">
         <v>1</v>
@@ -1128,22 +1136,22 @@
       <c r="D17" s="5">
         <v>37.5824</v>
       </c>
-      <c r="F17" s="26" t="s">
-        <v>5</v>
+      <c r="F17" s="38" t="s">
+        <v>4</v>
       </c>
       <c r="G17" s="4">
         <v>1</v>
       </c>
       <c r="H17" s="5"/>
-      <c r="J17" s="26" t="s">
-        <v>5</v>
+      <c r="J17" s="38" t="s">
+        <v>4</v>
       </c>
       <c r="K17" s="4">
         <v>1</v>
       </c>
       <c r="L17" s="5"/>
-      <c r="N17" s="26" t="s">
-        <v>5</v>
+      <c r="N17" s="38" t="s">
+        <v>4</v>
       </c>
       <c r="O17" s="4">
         <v>1</v>
@@ -1151,96 +1159,96 @@
       <c r="P17" s="5"/>
     </row>
     <row r="18" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B18" s="27"/>
+      <c r="B18" s="39"/>
       <c r="C18" s="6">
         <v>2</v>
       </c>
       <c r="D18" s="7">
         <v>37.5227</v>
       </c>
-      <c r="F18" s="27"/>
+      <c r="F18" s="39"/>
       <c r="G18" s="6">
         <v>2</v>
       </c>
       <c r="H18" s="7"/>
-      <c r="J18" s="27"/>
+      <c r="J18" s="39"/>
       <c r="K18" s="6">
         <v>2</v>
       </c>
       <c r="L18" s="7"/>
-      <c r="N18" s="27"/>
+      <c r="N18" s="39"/>
       <c r="O18" s="6">
         <v>2</v>
       </c>
       <c r="P18" s="7"/>
     </row>
     <row r="19" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B19" s="27"/>
+      <c r="B19" s="39"/>
       <c r="C19" s="6">
         <v>3</v>
       </c>
       <c r="D19" s="7">
         <v>37.150199999999998</v>
       </c>
-      <c r="F19" s="27"/>
+      <c r="F19" s="39"/>
       <c r="G19" s="6">
         <v>3</v>
       </c>
       <c r="H19" s="7"/>
-      <c r="J19" s="27"/>
+      <c r="J19" s="39"/>
       <c r="K19" s="6">
         <v>3</v>
       </c>
       <c r="L19" s="7"/>
-      <c r="N19" s="27"/>
+      <c r="N19" s="39"/>
       <c r="O19" s="6">
         <v>3</v>
       </c>
       <c r="P19" s="7"/>
     </row>
     <row r="20" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B20" s="27"/>
+      <c r="B20" s="39"/>
       <c r="C20" s="6">
         <v>4</v>
       </c>
       <c r="D20" s="7">
         <v>37.191299999999998</v>
       </c>
-      <c r="F20" s="27"/>
+      <c r="F20" s="39"/>
       <c r="G20" s="6">
         <v>4</v>
       </c>
       <c r="H20" s="7"/>
-      <c r="J20" s="27"/>
+      <c r="J20" s="39"/>
       <c r="K20" s="6">
         <v>4</v>
       </c>
       <c r="L20" s="7"/>
-      <c r="N20" s="27"/>
+      <c r="N20" s="39"/>
       <c r="O20" s="6">
         <v>4</v>
       </c>
       <c r="P20" s="7"/>
     </row>
     <row r="21" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="28"/>
+      <c r="B21" s="40"/>
       <c r="C21" s="8">
         <v>5</v>
       </c>
       <c r="D21" s="9">
         <v>39.039700000000003</v>
       </c>
-      <c r="F21" s="28"/>
+      <c r="F21" s="40"/>
       <c r="G21" s="8">
         <v>5</v>
       </c>
       <c r="H21" s="9"/>
-      <c r="J21" s="28"/>
+      <c r="J21" s="40"/>
       <c r="K21" s="8">
         <v>5</v>
       </c>
       <c r="L21" s="9"/>
-      <c r="N21" s="28"/>
+      <c r="N21" s="40"/>
       <c r="O21" s="8">
         <v>5</v>
       </c>
@@ -1287,8 +1295,8 @@
       <c r="P23" s="20"/>
     </row>
     <row r="24" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="26" t="s">
-        <v>6</v>
+      <c r="B24" s="38" t="s">
+        <v>5</v>
       </c>
       <c r="C24" s="4">
         <v>1</v>
@@ -1296,22 +1304,22 @@
       <c r="D24" s="5">
         <v>8.2642000000000007</v>
       </c>
-      <c r="F24" s="26" t="s">
-        <v>6</v>
+      <c r="F24" s="38" t="s">
+        <v>5</v>
       </c>
       <c r="G24" s="4">
         <v>1</v>
       </c>
       <c r="H24" s="5"/>
-      <c r="J24" s="26" t="s">
-        <v>6</v>
+      <c r="J24" s="38" t="s">
+        <v>5</v>
       </c>
       <c r="K24" s="4">
         <v>1</v>
       </c>
       <c r="L24" s="5"/>
-      <c r="N24" s="26" t="s">
-        <v>6</v>
+      <c r="N24" s="38" t="s">
+        <v>5</v>
       </c>
       <c r="O24" s="4">
         <v>1</v>
@@ -1319,96 +1327,96 @@
       <c r="P24" s="5"/>
     </row>
     <row r="25" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B25" s="27"/>
+      <c r="B25" s="39"/>
       <c r="C25" s="6">
         <v>2</v>
       </c>
       <c r="D25" s="7">
         <v>7.4324000000000003</v>
       </c>
-      <c r="F25" s="27"/>
+      <c r="F25" s="39"/>
       <c r="G25" s="6">
         <v>2</v>
       </c>
       <c r="H25" s="7"/>
-      <c r="J25" s="27"/>
+      <c r="J25" s="39"/>
       <c r="K25" s="6">
         <v>2</v>
       </c>
       <c r="L25" s="7"/>
-      <c r="N25" s="27"/>
+      <c r="N25" s="39"/>
       <c r="O25" s="6">
         <v>2</v>
       </c>
       <c r="P25" s="7"/>
     </row>
     <row r="26" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B26" s="27"/>
+      <c r="B26" s="39"/>
       <c r="C26" s="6">
         <v>3</v>
       </c>
       <c r="D26" s="7">
         <v>7.1902999999999997</v>
       </c>
-      <c r="F26" s="27"/>
+      <c r="F26" s="39"/>
       <c r="G26" s="6">
         <v>3</v>
       </c>
       <c r="H26" s="7"/>
-      <c r="J26" s="27"/>
+      <c r="J26" s="39"/>
       <c r="K26" s="6">
         <v>3</v>
       </c>
       <c r="L26" s="7"/>
-      <c r="N26" s="27"/>
+      <c r="N26" s="39"/>
       <c r="O26" s="6">
         <v>3</v>
       </c>
       <c r="P26" s="7"/>
     </row>
     <row r="27" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B27" s="27"/>
+      <c r="B27" s="39"/>
       <c r="C27" s="6">
         <v>4</v>
       </c>
       <c r="D27" s="7">
         <v>7.7202000000000002</v>
       </c>
-      <c r="F27" s="27"/>
+      <c r="F27" s="39"/>
       <c r="G27" s="6">
         <v>4</v>
       </c>
       <c r="H27" s="7"/>
-      <c r="J27" s="27"/>
+      <c r="J27" s="39"/>
       <c r="K27" s="6">
         <v>4</v>
       </c>
       <c r="L27" s="7"/>
-      <c r="N27" s="27"/>
+      <c r="N27" s="39"/>
       <c r="O27" s="6">
         <v>4</v>
       </c>
       <c r="P27" s="7"/>
     </row>
     <row r="28" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="28"/>
+      <c r="B28" s="40"/>
       <c r="C28" s="8">
         <v>5</v>
       </c>
       <c r="D28" s="9">
         <v>7.5617000000000001</v>
       </c>
-      <c r="F28" s="28"/>
+      <c r="F28" s="40"/>
       <c r="G28" s="8">
         <v>5</v>
       </c>
       <c r="H28" s="9"/>
-      <c r="J28" s="28"/>
+      <c r="J28" s="40"/>
       <c r="K28" s="8">
         <v>5</v>
       </c>
       <c r="L28" s="9"/>
-      <c r="N28" s="28"/>
+      <c r="N28" s="40"/>
       <c r="O28" s="8">
         <v>5</v>
       </c>
@@ -1442,12 +1450,6 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="N8:P9"/>
-    <mergeCell ref="N10:N14"/>
-    <mergeCell ref="J17:J21"/>
-    <mergeCell ref="N17:N21"/>
-    <mergeCell ref="J24:J28"/>
-    <mergeCell ref="N24:N28"/>
     <mergeCell ref="C2:K2"/>
     <mergeCell ref="B10:B14"/>
     <mergeCell ref="B17:B21"/>
@@ -1459,6 +1461,12 @@
     <mergeCell ref="B8:D9"/>
     <mergeCell ref="F8:H9"/>
     <mergeCell ref="J8:L9"/>
+    <mergeCell ref="N8:P9"/>
+    <mergeCell ref="N10:N14"/>
+    <mergeCell ref="J17:J21"/>
+    <mergeCell ref="N17:N21"/>
+    <mergeCell ref="J24:J28"/>
+    <mergeCell ref="N24:N28"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Added Testing Results for 10k Elements
</commit_message>
<xml_diff>
--- a/z_HybridAlgorithmResults.xlsx
+++ b/z_HybridAlgorithmResults.xlsx
@@ -504,6 +504,9 @@
     <xf numFmtId="3" fontId="1" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -513,6 +516,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -520,18 +532,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -817,7 +817,7 @@
   <dimension ref="B1:P29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17:F21"/>
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -829,20 +829,20 @@
     <row r="1" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="2"/>
-      <c r="C2" s="32" t="s">
+      <c r="C2" s="33" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="33"/>
-      <c r="E2" s="33"/>
-      <c r="F2" s="33"/>
-      <c r="G2" s="33"/>
-      <c r="H2" s="33"/>
-      <c r="I2" s="33"/>
-      <c r="J2" s="33"/>
-      <c r="K2" s="34"/>
+      <c r="D2" s="34"/>
+      <c r="E2" s="34"/>
+      <c r="F2" s="34"/>
+      <c r="G2" s="34"/>
+      <c r="H2" s="34"/>
+      <c r="I2" s="34"/>
+      <c r="J2" s="34"/>
+      <c r="K2" s="35"/>
     </row>
     <row r="3" spans="2:16" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="41" t="s">
+      <c r="B3" s="32" t="s">
         <v>11</v>
       </c>
       <c r="C3" s="27">
@@ -880,7 +880,9 @@
       <c r="C4" s="28">
         <v>2.6657999999999999</v>
       </c>
-      <c r="D4" s="29"/>
+      <c r="D4" s="29">
+        <v>5.8983800000000004</v>
+      </c>
       <c r="E4" s="29"/>
       <c r="F4" s="29"/>
       <c r="G4" s="29"/>
@@ -896,7 +898,9 @@
       <c r="C5" s="15">
         <v>37.69726</v>
       </c>
-      <c r="D5" s="11"/>
+      <c r="D5" s="11">
+        <v>152.03659999999999</v>
+      </c>
       <c r="E5" s="11"/>
       <c r="F5" s="11"/>
       <c r="G5" s="11"/>
@@ -912,7 +916,9 @@
       <c r="C6" s="17">
         <v>7.6337600000000005</v>
       </c>
-      <c r="D6" s="18"/>
+      <c r="D6" s="18">
+        <v>24.58466</v>
+      </c>
       <c r="E6" s="18"/>
       <c r="F6" s="18"/>
       <c r="G6" s="18"/>
@@ -923,43 +929,43 @@
     </row>
     <row r="7" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="8" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B8" s="32" t="s">
+      <c r="B8" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="33"/>
-      <c r="D8" s="34"/>
-      <c r="F8" s="32" t="s">
+      <c r="C8" s="34"/>
+      <c r="D8" s="35"/>
+      <c r="F8" s="33" t="s">
         <v>7</v>
       </c>
-      <c r="G8" s="33"/>
-      <c r="H8" s="34"/>
-      <c r="J8" s="32" t="s">
+      <c r="G8" s="34"/>
+      <c r="H8" s="35"/>
+      <c r="J8" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="K8" s="33"/>
-      <c r="L8" s="34"/>
-      <c r="N8" s="32" t="s">
+      <c r="K8" s="34"/>
+      <c r="L8" s="35"/>
+      <c r="N8" s="33" t="s">
         <v>9</v>
       </c>
-      <c r="O8" s="33"/>
-      <c r="P8" s="34"/>
+      <c r="O8" s="34"/>
+      <c r="P8" s="35"/>
     </row>
     <row r="9" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="35"/>
-      <c r="C9" s="36"/>
-      <c r="D9" s="37"/>
-      <c r="F9" s="35"/>
-      <c r="G9" s="36"/>
-      <c r="H9" s="37"/>
-      <c r="J9" s="35"/>
-      <c r="K9" s="36"/>
-      <c r="L9" s="37"/>
-      <c r="N9" s="35"/>
-      <c r="O9" s="36"/>
-      <c r="P9" s="37"/>
+      <c r="B9" s="39"/>
+      <c r="C9" s="40"/>
+      <c r="D9" s="41"/>
+      <c r="F9" s="39"/>
+      <c r="G9" s="40"/>
+      <c r="H9" s="41"/>
+      <c r="J9" s="39"/>
+      <c r="K9" s="40"/>
+      <c r="L9" s="41"/>
+      <c r="N9" s="39"/>
+      <c r="O9" s="40"/>
+      <c r="P9" s="41"/>
     </row>
     <row r="10" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="38" t="s">
+      <c r="B10" s="36" t="s">
         <v>3</v>
       </c>
       <c r="C10" s="4">
@@ -968,21 +974,23 @@
       <c r="D10" s="5">
         <v>2.6745999999999999</v>
       </c>
-      <c r="F10" s="38" t="s">
+      <c r="F10" s="36" t="s">
         <v>3</v>
       </c>
       <c r="G10" s="4">
         <v>1</v>
       </c>
-      <c r="H10" s="5"/>
-      <c r="J10" s="38" t="s">
+      <c r="H10" s="5">
+        <v>7.5720999999999998</v>
+      </c>
+      <c r="J10" s="36" t="s">
         <v>3</v>
       </c>
       <c r="K10" s="4">
         <v>1</v>
       </c>
       <c r="L10" s="5"/>
-      <c r="N10" s="38" t="s">
+      <c r="N10" s="36" t="s">
         <v>3</v>
       </c>
       <c r="O10" s="4">
@@ -991,96 +999,104 @@
       <c r="P10" s="5"/>
     </row>
     <row r="11" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B11" s="39"/>
+      <c r="B11" s="37"/>
       <c r="C11" s="6">
         <v>2</v>
       </c>
       <c r="D11" s="7">
         <v>2.6539999999999999</v>
       </c>
-      <c r="F11" s="39"/>
+      <c r="F11" s="37"/>
       <c r="G11" s="6">
         <v>2</v>
       </c>
-      <c r="H11" s="7"/>
-      <c r="J11" s="39"/>
+      <c r="H11" s="7">
+        <v>5.3691000000000004</v>
+      </c>
+      <c r="J11" s="37"/>
       <c r="K11" s="6">
         <v>2</v>
       </c>
       <c r="L11" s="7"/>
-      <c r="N11" s="39"/>
+      <c r="N11" s="37"/>
       <c r="O11" s="6">
         <v>2</v>
       </c>
       <c r="P11" s="7"/>
     </row>
     <row r="12" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B12" s="39"/>
+      <c r="B12" s="37"/>
       <c r="C12" s="6">
         <v>3</v>
       </c>
       <c r="D12" s="7">
         <v>2.6448</v>
       </c>
-      <c r="F12" s="39"/>
+      <c r="F12" s="37"/>
       <c r="G12" s="6">
         <v>3</v>
       </c>
-      <c r="H12" s="7"/>
-      <c r="J12" s="39"/>
+      <c r="H12" s="7">
+        <v>5.5719000000000003</v>
+      </c>
+      <c r="J12" s="37"/>
       <c r="K12" s="6">
         <v>3</v>
       </c>
       <c r="L12" s="7"/>
-      <c r="N12" s="39"/>
+      <c r="N12" s="37"/>
       <c r="O12" s="6">
         <v>3</v>
       </c>
       <c r="P12" s="7"/>
     </row>
     <row r="13" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B13" s="39"/>
+      <c r="B13" s="37"/>
       <c r="C13" s="6">
         <v>4</v>
       </c>
       <c r="D13" s="7">
         <v>2.6669999999999998</v>
       </c>
-      <c r="F13" s="39"/>
+      <c r="F13" s="37"/>
       <c r="G13" s="6">
         <v>4</v>
       </c>
-      <c r="H13" s="7"/>
-      <c r="J13" s="39"/>
+      <c r="H13" s="7">
+        <v>5.3932000000000002</v>
+      </c>
+      <c r="J13" s="37"/>
       <c r="K13" s="6">
         <v>4</v>
       </c>
       <c r="L13" s="7"/>
-      <c r="N13" s="39"/>
+      <c r="N13" s="37"/>
       <c r="O13" s="6">
         <v>4</v>
       </c>
       <c r="P13" s="7"/>
     </row>
     <row r="14" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="40"/>
+      <c r="B14" s="38"/>
       <c r="C14" s="8">
         <v>5</v>
       </c>
       <c r="D14" s="9">
         <v>2.6886000000000001</v>
       </c>
-      <c r="F14" s="40"/>
+      <c r="F14" s="38"/>
       <c r="G14" s="8">
         <v>5</v>
       </c>
-      <c r="H14" s="9"/>
-      <c r="J14" s="40"/>
+      <c r="H14" s="9">
+        <v>5.5856000000000003</v>
+      </c>
+      <c r="J14" s="38"/>
       <c r="K14" s="8">
         <v>5</v>
       </c>
       <c r="L14" s="9"/>
-      <c r="N14" s="40"/>
+      <c r="N14" s="38"/>
       <c r="O14" s="8">
         <v>5</v>
       </c>
@@ -1095,9 +1111,9 @@
       </c>
       <c r="F15" s="3"/>
       <c r="G15" s="21"/>
-      <c r="H15" s="10" t="e">
+      <c r="H15" s="10">
         <f>AVERAGE(H10:H14)</f>
-        <v>#DIV/0!</v>
+        <v>5.8983800000000004</v>
       </c>
       <c r="J15" s="3"/>
       <c r="K15" s="21"/>
@@ -1127,7 +1143,7 @@
       <c r="P16" s="20"/>
     </row>
     <row r="17" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="38" t="s">
+      <c r="B17" s="36" t="s">
         <v>4</v>
       </c>
       <c r="C17" s="4">
@@ -1136,21 +1152,23 @@
       <c r="D17" s="5">
         <v>37.5824</v>
       </c>
-      <c r="F17" s="38" t="s">
+      <c r="F17" s="36" t="s">
         <v>4</v>
       </c>
       <c r="G17" s="4">
         <v>1</v>
       </c>
-      <c r="H17" s="5"/>
-      <c r="J17" s="38" t="s">
+      <c r="H17" s="5">
+        <v>150.71100000000001</v>
+      </c>
+      <c r="J17" s="36" t="s">
         <v>4</v>
       </c>
       <c r="K17" s="4">
         <v>1</v>
       </c>
       <c r="L17" s="5"/>
-      <c r="N17" s="38" t="s">
+      <c r="N17" s="36" t="s">
         <v>4</v>
       </c>
       <c r="O17" s="4">
@@ -1159,96 +1177,104 @@
       <c r="P17" s="5"/>
     </row>
     <row r="18" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B18" s="39"/>
+      <c r="B18" s="37"/>
       <c r="C18" s="6">
         <v>2</v>
       </c>
       <c r="D18" s="7">
         <v>37.5227</v>
       </c>
-      <c r="F18" s="39"/>
+      <c r="F18" s="37"/>
       <c r="G18" s="6">
         <v>2</v>
       </c>
-      <c r="H18" s="7"/>
-      <c r="J18" s="39"/>
+      <c r="H18" s="7">
+        <v>151.33600000000001</v>
+      </c>
+      <c r="J18" s="37"/>
       <c r="K18" s="6">
         <v>2</v>
       </c>
       <c r="L18" s="7"/>
-      <c r="N18" s="39"/>
+      <c r="N18" s="37"/>
       <c r="O18" s="6">
         <v>2</v>
       </c>
       <c r="P18" s="7"/>
     </row>
     <row r="19" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B19" s="39"/>
+      <c r="B19" s="37"/>
       <c r="C19" s="6">
         <v>3</v>
       </c>
       <c r="D19" s="7">
         <v>37.150199999999998</v>
       </c>
-      <c r="F19" s="39"/>
+      <c r="F19" s="37"/>
       <c r="G19" s="6">
         <v>3</v>
       </c>
-      <c r="H19" s="7"/>
-      <c r="J19" s="39"/>
+      <c r="H19" s="7">
+        <v>150.72900000000001</v>
+      </c>
+      <c r="J19" s="37"/>
       <c r="K19" s="6">
         <v>3</v>
       </c>
       <c r="L19" s="7"/>
-      <c r="N19" s="39"/>
+      <c r="N19" s="37"/>
       <c r="O19" s="6">
         <v>3</v>
       </c>
       <c r="P19" s="7"/>
     </row>
     <row r="20" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B20" s="39"/>
+      <c r="B20" s="37"/>
       <c r="C20" s="6">
         <v>4</v>
       </c>
       <c r="D20" s="7">
         <v>37.191299999999998</v>
       </c>
-      <c r="F20" s="39"/>
+      <c r="F20" s="37"/>
       <c r="G20" s="6">
         <v>4</v>
       </c>
-      <c r="H20" s="7"/>
-      <c r="J20" s="39"/>
+      <c r="H20" s="7">
+        <v>158.339</v>
+      </c>
+      <c r="J20" s="37"/>
       <c r="K20" s="6">
         <v>4</v>
       </c>
       <c r="L20" s="7"/>
-      <c r="N20" s="39"/>
+      <c r="N20" s="37"/>
       <c r="O20" s="6">
         <v>4</v>
       </c>
       <c r="P20" s="7"/>
     </row>
     <row r="21" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="40"/>
+      <c r="B21" s="38"/>
       <c r="C21" s="8">
         <v>5</v>
       </c>
       <c r="D21" s="9">
         <v>39.039700000000003</v>
       </c>
-      <c r="F21" s="40"/>
+      <c r="F21" s="38"/>
       <c r="G21" s="8">
         <v>5</v>
       </c>
-      <c r="H21" s="9"/>
-      <c r="J21" s="40"/>
+      <c r="H21" s="9">
+        <v>149.06800000000001</v>
+      </c>
+      <c r="J21" s="38"/>
       <c r="K21" s="8">
         <v>5</v>
       </c>
       <c r="L21" s="9"/>
-      <c r="N21" s="40"/>
+      <c r="N21" s="38"/>
       <c r="O21" s="8">
         <v>5</v>
       </c>
@@ -1263,9 +1289,9 @@
       </c>
       <c r="F22" s="3"/>
       <c r="G22" s="21"/>
-      <c r="H22" s="10" t="e">
+      <c r="H22" s="10">
         <f>AVERAGE(H17:H21)</f>
-        <v>#DIV/0!</v>
+        <v>152.03659999999999</v>
       </c>
       <c r="J22" s="3"/>
       <c r="K22" s="21"/>
@@ -1295,7 +1321,7 @@
       <c r="P23" s="20"/>
     </row>
     <row r="24" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="38" t="s">
+      <c r="B24" s="36" t="s">
         <v>5</v>
       </c>
       <c r="C24" s="4">
@@ -1304,21 +1330,23 @@
       <c r="D24" s="5">
         <v>8.2642000000000007</v>
       </c>
-      <c r="F24" s="38" t="s">
+      <c r="F24" s="36" t="s">
         <v>5</v>
       </c>
       <c r="G24" s="4">
         <v>1</v>
       </c>
-      <c r="H24" s="5"/>
-      <c r="J24" s="38" t="s">
+      <c r="H24" s="5">
+        <v>25.076599999999999</v>
+      </c>
+      <c r="J24" s="36" t="s">
         <v>5</v>
       </c>
       <c r="K24" s="4">
         <v>1</v>
       </c>
       <c r="L24" s="5"/>
-      <c r="N24" s="38" t="s">
+      <c r="N24" s="36" t="s">
         <v>5</v>
       </c>
       <c r="O24" s="4">
@@ -1327,96 +1355,104 @@
       <c r="P24" s="5"/>
     </row>
     <row r="25" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B25" s="39"/>
+      <c r="B25" s="37"/>
       <c r="C25" s="6">
         <v>2</v>
       </c>
       <c r="D25" s="7">
         <v>7.4324000000000003</v>
       </c>
-      <c r="F25" s="39"/>
+      <c r="F25" s="37"/>
       <c r="G25" s="6">
         <v>2</v>
       </c>
-      <c r="H25" s="7"/>
-      <c r="J25" s="39"/>
+      <c r="H25" s="7">
+        <v>24.748200000000001</v>
+      </c>
+      <c r="J25" s="37"/>
       <c r="K25" s="6">
         <v>2</v>
       </c>
       <c r="L25" s="7"/>
-      <c r="N25" s="39"/>
+      <c r="N25" s="37"/>
       <c r="O25" s="6">
         <v>2</v>
       </c>
       <c r="P25" s="7"/>
     </row>
     <row r="26" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B26" s="39"/>
+      <c r="B26" s="37"/>
       <c r="C26" s="6">
         <v>3</v>
       </c>
       <c r="D26" s="7">
         <v>7.1902999999999997</v>
       </c>
-      <c r="F26" s="39"/>
+      <c r="F26" s="37"/>
       <c r="G26" s="6">
         <v>3</v>
       </c>
-      <c r="H26" s="7"/>
-      <c r="J26" s="39"/>
+      <c r="H26" s="7">
+        <v>24.3325</v>
+      </c>
+      <c r="J26" s="37"/>
       <c r="K26" s="6">
         <v>3</v>
       </c>
       <c r="L26" s="7"/>
-      <c r="N26" s="39"/>
+      <c r="N26" s="37"/>
       <c r="O26" s="6">
         <v>3</v>
       </c>
       <c r="P26" s="7"/>
     </row>
     <row r="27" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B27" s="39"/>
+      <c r="B27" s="37"/>
       <c r="C27" s="6">
         <v>4</v>
       </c>
       <c r="D27" s="7">
         <v>7.7202000000000002</v>
       </c>
-      <c r="F27" s="39"/>
+      <c r="F27" s="37"/>
       <c r="G27" s="6">
         <v>4</v>
       </c>
-      <c r="H27" s="7"/>
-      <c r="J27" s="39"/>
+      <c r="H27" s="7">
+        <v>24.497900000000001</v>
+      </c>
+      <c r="J27" s="37"/>
       <c r="K27" s="6">
         <v>4</v>
       </c>
       <c r="L27" s="7"/>
-      <c r="N27" s="39"/>
+      <c r="N27" s="37"/>
       <c r="O27" s="6">
         <v>4</v>
       </c>
       <c r="P27" s="7"/>
     </row>
     <row r="28" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="40"/>
+      <c r="B28" s="38"/>
       <c r="C28" s="8">
         <v>5</v>
       </c>
       <c r="D28" s="9">
         <v>7.5617000000000001</v>
       </c>
-      <c r="F28" s="40"/>
+      <c r="F28" s="38"/>
       <c r="G28" s="8">
         <v>5</v>
       </c>
-      <c r="H28" s="9"/>
-      <c r="J28" s="40"/>
+      <c r="H28" s="9">
+        <v>24.2681</v>
+      </c>
+      <c r="J28" s="38"/>
       <c r="K28" s="8">
         <v>5</v>
       </c>
       <c r="L28" s="9"/>
-      <c r="N28" s="40"/>
+      <c r="N28" s="38"/>
       <c r="O28" s="8">
         <v>5</v>
       </c>
@@ -1431,9 +1467,9 @@
       </c>
       <c r="F29" s="24"/>
       <c r="G29" s="25"/>
-      <c r="H29" s="10" t="e">
+      <c r="H29" s="10">
         <f>AVERAGE(H24:H28)</f>
-        <v>#DIV/0!</v>
+        <v>24.58466</v>
       </c>
       <c r="J29" s="24"/>
       <c r="K29" s="25"/>
@@ -1450,6 +1486,12 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="N8:P9"/>
+    <mergeCell ref="N10:N14"/>
+    <mergeCell ref="J17:J21"/>
+    <mergeCell ref="N17:N21"/>
+    <mergeCell ref="J24:J28"/>
+    <mergeCell ref="N24:N28"/>
     <mergeCell ref="C2:K2"/>
     <mergeCell ref="B10:B14"/>
     <mergeCell ref="B17:B21"/>
@@ -1461,12 +1503,6 @@
     <mergeCell ref="B8:D9"/>
     <mergeCell ref="F8:H9"/>
     <mergeCell ref="J8:L9"/>
-    <mergeCell ref="N8:P9"/>
-    <mergeCell ref="N10:N14"/>
-    <mergeCell ref="J17:J21"/>
-    <mergeCell ref="N17:N21"/>
-    <mergeCell ref="J24:J28"/>
-    <mergeCell ref="N24:N28"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Added test results for 35k and 40k elements
</commit_message>
<xml_diff>
--- a/z_HybridAlgorithmResults.xlsx
+++ b/z_HybridAlgorithmResults.xlsx
@@ -459,7 +459,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -540,6 +540,12 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="1" fontId="2" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -587,6 +593,1151 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Hybrid</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$C$3:$K$3</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>15000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>20000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>25000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>30000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>35000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>40000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>45000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$C$4:$K$4</c:f>
+              <c:numCache>
+                <c:formatCode>0.0000</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>2.6657999999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.8983800000000004</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8.2913399999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>11.956979999999998</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>15.996119999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>16.98348</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>16.532519999999998</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>20.424439999999997</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Bubble</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$C$3:$K$3</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>15000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>20000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>25000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>30000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>35000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>40000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>45000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$C$5:$K$5</c:f>
+              <c:numCache>
+                <c:formatCode>0.0000</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>37.69726</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>152.03659999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>353.97480000000002</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>672.91099999999994</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1138.066</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1739.6299999999999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2455.018</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3308.5839999999998</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$6</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Merge</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$C$3:$K$3</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>15000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>20000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>25000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>30000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>35000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>40000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>45000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$C$6:$K$6</c:f>
+              <c:numCache>
+                <c:formatCode>0.0000</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>7.6337600000000005</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>24.58466</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>33.474100000000007</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>85.974559999999997</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>106.2856</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>119.79220000000001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>425.20439999999996</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>427.07280000000003</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="402435584"/>
+        <c:axId val="402436128"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="402435584"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="402436128"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="402436128"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.0000" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="402435584"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>78441</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>68355</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>414618</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>88525</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -877,10 +2028,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:P52"/>
+  <dimension ref="A1:P53"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="S17" sqref="S17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -897,17 +2048,17 @@
     <row r="1" spans="2:16" ht="24" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:16" s="1" customFormat="1" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="3"/>
-      <c r="C2" s="32" t="s">
+      <c r="C2" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="33"/>
-      <c r="E2" s="33"/>
-      <c r="F2" s="33"/>
-      <c r="G2" s="33"/>
-      <c r="H2" s="33"/>
-      <c r="I2" s="33"/>
-      <c r="J2" s="33"/>
-      <c r="K2" s="34"/>
+      <c r="D2" s="35"/>
+      <c r="E2" s="35"/>
+      <c r="F2" s="35"/>
+      <c r="G2" s="35"/>
+      <c r="H2" s="35"/>
+      <c r="I2" s="35"/>
+      <c r="J2" s="35"/>
+      <c r="K2" s="36"/>
     </row>
     <row r="3" spans="2:16" s="1" customFormat="1" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="4" t="s">
@@ -963,8 +2114,12 @@
       <c r="H4" s="7">
         <v>16.98348</v>
       </c>
-      <c r="I4" s="7"/>
-      <c r="J4" s="7"/>
+      <c r="I4" s="7">
+        <v>16.532519999999998</v>
+      </c>
+      <c r="J4" s="7">
+        <v>20.424439999999997</v>
+      </c>
       <c r="K4" s="8"/>
     </row>
     <row r="5" spans="2:16" s="1" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
@@ -989,8 +2144,12 @@
       <c r="H5" s="11">
         <v>1739.6299999999999</v>
       </c>
-      <c r="I5" s="11"/>
-      <c r="J5" s="11"/>
+      <c r="I5" s="11">
+        <v>2455.018</v>
+      </c>
+      <c r="J5" s="11">
+        <v>3308.5839999999998</v>
+      </c>
       <c r="K5" s="12"/>
     </row>
     <row r="6" spans="2:16" s="1" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
@@ -1015,49 +2174,53 @@
       <c r="H6" s="15">
         <v>119.79220000000001</v>
       </c>
-      <c r="I6" s="15"/>
-      <c r="J6" s="15"/>
+      <c r="I6" s="15">
+        <v>425.20439999999996</v>
+      </c>
+      <c r="J6" s="15">
+        <v>427.07280000000003</v>
+      </c>
       <c r="K6" s="16"/>
     </row>
     <row r="7" spans="2:16" ht="24" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="8" spans="2:16" s="1" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="32" t="s">
+      <c r="B8" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="33"/>
-      <c r="D8" s="34"/>
-      <c r="F8" s="32" t="s">
+      <c r="C8" s="35"/>
+      <c r="D8" s="36"/>
+      <c r="F8" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="G8" s="33"/>
-      <c r="H8" s="34"/>
-      <c r="J8" s="32" t="s">
+      <c r="G8" s="35"/>
+      <c r="H8" s="36"/>
+      <c r="J8" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="K8" s="33"/>
-      <c r="L8" s="34"/>
-      <c r="N8" s="32" t="s">
+      <c r="K8" s="35"/>
+      <c r="L8" s="36"/>
+      <c r="N8" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="O8" s="33"/>
-      <c r="P8" s="34"/>
+      <c r="O8" s="35"/>
+      <c r="P8" s="36"/>
     </row>
     <row r="9" spans="2:16" s="1" customFormat="1" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="35"/>
-      <c r="C9" s="36"/>
-      <c r="D9" s="37"/>
-      <c r="F9" s="35"/>
-      <c r="G9" s="36"/>
-      <c r="H9" s="37"/>
-      <c r="J9" s="35"/>
-      <c r="K9" s="36"/>
-      <c r="L9" s="37"/>
-      <c r="N9" s="35"/>
-      <c r="O9" s="36"/>
-      <c r="P9" s="37"/>
+      <c r="B9" s="37"/>
+      <c r="C9" s="38"/>
+      <c r="D9" s="39"/>
+      <c r="F9" s="37"/>
+      <c r="G9" s="38"/>
+      <c r="H9" s="39"/>
+      <c r="J9" s="37"/>
+      <c r="K9" s="38"/>
+      <c r="L9" s="39"/>
+      <c r="N9" s="37"/>
+      <c r="O9" s="38"/>
+      <c r="P9" s="39"/>
     </row>
     <row r="10" spans="2:16" s="1" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="28" t="s">
+      <c r="B10" s="30" t="s">
         <v>9</v>
       </c>
       <c r="C10" s="23">
@@ -1066,7 +2229,7 @@
       <c r="D10" s="17">
         <v>2.6745999999999999</v>
       </c>
-      <c r="F10" s="28" t="s">
+      <c r="F10" s="30" t="s">
         <v>9</v>
       </c>
       <c r="G10" s="23">
@@ -1075,7 +2238,7 @@
       <c r="H10" s="17">
         <v>7.5720999999999998</v>
       </c>
-      <c r="J10" s="28" t="s">
+      <c r="J10" s="30" t="s">
         <v>9</v>
       </c>
       <c r="K10" s="23">
@@ -1084,7 +2247,7 @@
       <c r="L10" s="17">
         <v>8.4957999999999991</v>
       </c>
-      <c r="N10" s="28" t="s">
+      <c r="N10" s="30" t="s">
         <v>9</v>
       </c>
       <c r="O10" s="23">
@@ -1095,28 +2258,28 @@
       </c>
     </row>
     <row r="11" spans="2:16" s="1" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="29"/>
+      <c r="B11" s="31"/>
       <c r="C11" s="24">
         <v>2</v>
       </c>
       <c r="D11" s="19">
         <v>2.6539999999999999</v>
       </c>
-      <c r="F11" s="29"/>
+      <c r="F11" s="31"/>
       <c r="G11" s="24">
         <v>2</v>
       </c>
       <c r="H11" s="19">
         <v>5.3691000000000004</v>
       </c>
-      <c r="J11" s="29"/>
+      <c r="J11" s="31"/>
       <c r="K11" s="24">
         <v>2</v>
       </c>
       <c r="L11" s="19">
         <v>8.4400999999999993</v>
       </c>
-      <c r="N11" s="29"/>
+      <c r="N11" s="31"/>
       <c r="O11" s="24">
         <v>2</v>
       </c>
@@ -1125,28 +2288,28 @@
       </c>
     </row>
     <row r="12" spans="2:16" s="1" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="29"/>
+      <c r="B12" s="31"/>
       <c r="C12" s="24">
         <v>3</v>
       </c>
       <c r="D12" s="19">
         <v>2.6448</v>
       </c>
-      <c r="F12" s="29"/>
+      <c r="F12" s="31"/>
       <c r="G12" s="24">
         <v>3</v>
       </c>
       <c r="H12" s="19">
         <v>5.5719000000000003</v>
       </c>
-      <c r="J12" s="29"/>
+      <c r="J12" s="31"/>
       <c r="K12" s="24">
         <v>3</v>
       </c>
       <c r="L12" s="19">
         <v>8.2652999999999999</v>
       </c>
-      <c r="N12" s="29"/>
+      <c r="N12" s="31"/>
       <c r="O12" s="24">
         <v>3</v>
       </c>
@@ -1155,28 +2318,28 @@
       </c>
     </row>
     <row r="13" spans="2:16" s="1" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="29"/>
+      <c r="B13" s="31"/>
       <c r="C13" s="24">
         <v>4</v>
       </c>
       <c r="D13" s="19">
         <v>2.6669999999999998</v>
       </c>
-      <c r="F13" s="29"/>
+      <c r="F13" s="31"/>
       <c r="G13" s="24">
         <v>4</v>
       </c>
       <c r="H13" s="19">
         <v>5.3932000000000002</v>
       </c>
-      <c r="J13" s="29"/>
+      <c r="J13" s="31"/>
       <c r="K13" s="24">
         <v>4</v>
       </c>
       <c r="L13" s="19">
         <v>8.1226000000000003</v>
       </c>
-      <c r="N13" s="29"/>
+      <c r="N13" s="31"/>
       <c r="O13" s="24">
         <v>4</v>
       </c>
@@ -1185,28 +2348,28 @@
       </c>
     </row>
     <row r="14" spans="2:16" s="1" customFormat="1" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="29"/>
+      <c r="B14" s="31"/>
       <c r="C14" s="24">
         <v>5</v>
       </c>
       <c r="D14" s="20">
         <v>2.6886000000000001</v>
       </c>
-      <c r="F14" s="29"/>
+      <c r="F14" s="31"/>
       <c r="G14" s="24">
         <v>5</v>
       </c>
       <c r="H14" s="20">
         <v>5.5856000000000003</v>
       </c>
-      <c r="J14" s="29"/>
+      <c r="J14" s="31"/>
       <c r="K14" s="24">
         <v>5</v>
       </c>
       <c r="L14" s="20">
         <v>8.1328999999999994</v>
       </c>
-      <c r="N14" s="29"/>
+      <c r="N14" s="31"/>
       <c r="O14" s="24">
         <v>5</v>
       </c>
@@ -1215,34 +2378,34 @@
       </c>
     </row>
     <row r="15" spans="2:16" s="1" customFormat="1" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="30" t="s">
+      <c r="B15" s="32" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="31"/>
+      <c r="C15" s="33"/>
       <c r="D15" s="21">
         <f>AVERAGE(D10:D14)</f>
         <v>2.6657999999999999</v>
       </c>
-      <c r="F15" s="30" t="s">
+      <c r="F15" s="32" t="s">
         <v>12</v>
       </c>
-      <c r="G15" s="31"/>
+      <c r="G15" s="33"/>
       <c r="H15" s="21">
         <f>AVERAGE(H10:H14)</f>
         <v>5.8983800000000004</v>
       </c>
-      <c r="J15" s="30" t="s">
+      <c r="J15" s="32" t="s">
         <v>12</v>
       </c>
-      <c r="K15" s="31"/>
+      <c r="K15" s="33"/>
       <c r="L15" s="21">
         <f>AVERAGE(L10:L14)</f>
         <v>8.2913399999999999</v>
       </c>
-      <c r="N15" s="30" t="s">
+      <c r="N15" s="32" t="s">
         <v>12</v>
       </c>
-      <c r="O15" s="31"/>
+      <c r="O15" s="33"/>
       <c r="P15" s="21">
         <f>AVERAGE(P10:P14)</f>
         <v>11.956979999999998</v>
@@ -1263,7 +2426,7 @@
       <c r="P16" s="19"/>
     </row>
     <row r="17" spans="2:16" s="1" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="28" t="s">
+      <c r="B17" s="30" t="s">
         <v>10</v>
       </c>
       <c r="C17" s="23">
@@ -1272,7 +2435,7 @@
       <c r="D17" s="17">
         <v>37.5824</v>
       </c>
-      <c r="F17" s="28" t="s">
+      <c r="F17" s="30" t="s">
         <v>10</v>
       </c>
       <c r="G17" s="23">
@@ -1281,7 +2444,7 @@
       <c r="H17" s="17">
         <v>150.71100000000001</v>
       </c>
-      <c r="J17" s="28" t="s">
+      <c r="J17" s="30" t="s">
         <v>10</v>
       </c>
       <c r="K17" s="23">
@@ -1290,7 +2453,7 @@
       <c r="L17" s="17">
         <v>351.39299999999997</v>
       </c>
-      <c r="N17" s="28" t="s">
+      <c r="N17" s="30" t="s">
         <v>10</v>
       </c>
       <c r="O17" s="23">
@@ -1301,28 +2464,28 @@
       </c>
     </row>
     <row r="18" spans="2:16" s="1" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="29"/>
+      <c r="B18" s="31"/>
       <c r="C18" s="24">
         <v>2</v>
       </c>
       <c r="D18" s="19">
         <v>37.5227</v>
       </c>
-      <c r="F18" s="29"/>
+      <c r="F18" s="31"/>
       <c r="G18" s="24">
         <v>2</v>
       </c>
       <c r="H18" s="19">
         <v>151.33600000000001</v>
       </c>
-      <c r="J18" s="29"/>
+      <c r="J18" s="31"/>
       <c r="K18" s="24">
         <v>2</v>
       </c>
       <c r="L18" s="19">
         <v>352.65899999999999</v>
       </c>
-      <c r="N18" s="29"/>
+      <c r="N18" s="31"/>
       <c r="O18" s="24">
         <v>2</v>
       </c>
@@ -1331,28 +2494,28 @@
       </c>
     </row>
     <row r="19" spans="2:16" s="1" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="29"/>
+      <c r="B19" s="31"/>
       <c r="C19" s="24">
         <v>3</v>
       </c>
       <c r="D19" s="19">
         <v>37.150199999999998</v>
       </c>
-      <c r="F19" s="29"/>
+      <c r="F19" s="31"/>
       <c r="G19" s="24">
         <v>3</v>
       </c>
       <c r="H19" s="19">
         <v>150.72900000000001</v>
       </c>
-      <c r="J19" s="29"/>
+      <c r="J19" s="31"/>
       <c r="K19" s="24">
         <v>3</v>
       </c>
       <c r="L19" s="19">
         <v>355.22199999999998</v>
       </c>
-      <c r="N19" s="29"/>
+      <c r="N19" s="31"/>
       <c r="O19" s="24">
         <v>3</v>
       </c>
@@ -1361,28 +2524,28 @@
       </c>
     </row>
     <row r="20" spans="2:16" s="1" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="29"/>
+      <c r="B20" s="31"/>
       <c r="C20" s="24">
         <v>4</v>
       </c>
       <c r="D20" s="19">
         <v>37.191299999999998</v>
       </c>
-      <c r="F20" s="29"/>
+      <c r="F20" s="31"/>
       <c r="G20" s="24">
         <v>4</v>
       </c>
       <c r="H20" s="19">
         <v>158.339</v>
       </c>
-      <c r="J20" s="29"/>
+      <c r="J20" s="31"/>
       <c r="K20" s="24">
         <v>4</v>
       </c>
       <c r="L20" s="19">
         <v>354.48500000000001</v>
       </c>
-      <c r="N20" s="29"/>
+      <c r="N20" s="31"/>
       <c r="O20" s="24">
         <v>4</v>
       </c>
@@ -1391,28 +2554,28 @@
       </c>
     </row>
     <row r="21" spans="2:16" s="1" customFormat="1" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="29"/>
+      <c r="B21" s="31"/>
       <c r="C21" s="24">
         <v>5</v>
       </c>
       <c r="D21" s="20">
         <v>39.039700000000003</v>
       </c>
-      <c r="F21" s="29"/>
+      <c r="F21" s="31"/>
       <c r="G21" s="24">
         <v>5</v>
       </c>
       <c r="H21" s="20">
         <v>149.06800000000001</v>
       </c>
-      <c r="J21" s="29"/>
+      <c r="J21" s="31"/>
       <c r="K21" s="24">
         <v>5</v>
       </c>
       <c r="L21" s="20">
         <v>356.11500000000001</v>
       </c>
-      <c r="N21" s="29"/>
+      <c r="N21" s="31"/>
       <c r="O21" s="24">
         <v>5</v>
       </c>
@@ -1421,34 +2584,34 @@
       </c>
     </row>
     <row r="22" spans="2:16" s="1" customFormat="1" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="30" t="s">
+      <c r="B22" s="32" t="s">
         <v>12</v>
       </c>
-      <c r="C22" s="31"/>
+      <c r="C22" s="33"/>
       <c r="D22" s="21">
         <f>AVERAGE(D17:D21)</f>
         <v>37.69726</v>
       </c>
-      <c r="F22" s="30" t="s">
+      <c r="F22" s="32" t="s">
         <v>12</v>
       </c>
-      <c r="G22" s="31"/>
+      <c r="G22" s="33"/>
       <c r="H22" s="21">
         <f>AVERAGE(H17:H21)</f>
         <v>152.03659999999999</v>
       </c>
-      <c r="J22" s="30" t="s">
+      <c r="J22" s="32" t="s">
         <v>12</v>
       </c>
-      <c r="K22" s="31"/>
+      <c r="K22" s="33"/>
       <c r="L22" s="21">
         <f>AVERAGE(L17:L21)</f>
         <v>353.97480000000002</v>
       </c>
-      <c r="N22" s="30" t="s">
+      <c r="N22" s="32" t="s">
         <v>12</v>
       </c>
-      <c r="O22" s="31"/>
+      <c r="O22" s="33"/>
       <c r="P22" s="21">
         <f>AVERAGE(P17:P21)</f>
         <v>672.91099999999994</v>
@@ -1469,7 +2632,7 @@
       <c r="P23" s="19"/>
     </row>
     <row r="24" spans="2:16" s="1" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="28" t="s">
+      <c r="B24" s="30" t="s">
         <v>11</v>
       </c>
       <c r="C24" s="23">
@@ -1478,7 +2641,7 @@
       <c r="D24" s="17">
         <v>8.2642000000000007</v>
       </c>
-      <c r="F24" s="28" t="s">
+      <c r="F24" s="30" t="s">
         <v>11</v>
       </c>
       <c r="G24" s="23">
@@ -1487,7 +2650,7 @@
       <c r="H24" s="17">
         <v>25.076599999999999</v>
       </c>
-      <c r="J24" s="28" t="s">
+      <c r="J24" s="30" t="s">
         <v>11</v>
       </c>
       <c r="K24" s="23">
@@ -1496,7 +2659,7 @@
       <c r="L24" s="17">
         <v>34.4285</v>
       </c>
-      <c r="N24" s="28" t="s">
+      <c r="N24" s="30" t="s">
         <v>11</v>
       </c>
       <c r="O24" s="23">
@@ -1507,28 +2670,28 @@
       </c>
     </row>
     <row r="25" spans="2:16" s="1" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="29"/>
+      <c r="B25" s="31"/>
       <c r="C25" s="24">
         <v>2</v>
       </c>
       <c r="D25" s="19">
         <v>7.4324000000000003</v>
       </c>
-      <c r="F25" s="29"/>
+      <c r="F25" s="31"/>
       <c r="G25" s="24">
         <v>2</v>
       </c>
       <c r="H25" s="19">
         <v>24.748200000000001</v>
       </c>
-      <c r="J25" s="29"/>
+      <c r="J25" s="31"/>
       <c r="K25" s="24">
         <v>2</v>
       </c>
       <c r="L25" s="19">
         <v>33.139099999999999</v>
       </c>
-      <c r="N25" s="29"/>
+      <c r="N25" s="31"/>
       <c r="O25" s="24">
         <v>2</v>
       </c>
@@ -1537,28 +2700,28 @@
       </c>
     </row>
     <row r="26" spans="2:16" s="1" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="29"/>
+      <c r="B26" s="31"/>
       <c r="C26" s="24">
         <v>3</v>
       </c>
       <c r="D26" s="19">
         <v>7.1902999999999997</v>
       </c>
-      <c r="F26" s="29"/>
+      <c r="F26" s="31"/>
       <c r="G26" s="24">
         <v>3</v>
       </c>
       <c r="H26" s="19">
         <v>24.3325</v>
       </c>
-      <c r="J26" s="29"/>
+      <c r="J26" s="31"/>
       <c r="K26" s="24">
         <v>3</v>
       </c>
       <c r="L26" s="19">
         <v>33.017400000000002</v>
       </c>
-      <c r="N26" s="29"/>
+      <c r="N26" s="31"/>
       <c r="O26" s="24">
         <v>3</v>
       </c>
@@ -1567,28 +2730,28 @@
       </c>
     </row>
     <row r="27" spans="2:16" s="1" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="29"/>
+      <c r="B27" s="31"/>
       <c r="C27" s="24">
         <v>4</v>
       </c>
       <c r="D27" s="19">
         <v>7.7202000000000002</v>
       </c>
-      <c r="F27" s="29"/>
+      <c r="F27" s="31"/>
       <c r="G27" s="24">
         <v>4</v>
       </c>
       <c r="H27" s="19">
         <v>24.497900000000001</v>
       </c>
-      <c r="J27" s="29"/>
+      <c r="J27" s="31"/>
       <c r="K27" s="24">
         <v>4</v>
       </c>
       <c r="L27" s="19">
         <v>33.351999999999997</v>
       </c>
-      <c r="N27" s="29"/>
+      <c r="N27" s="31"/>
       <c r="O27" s="24">
         <v>4</v>
       </c>
@@ -1597,28 +2760,28 @@
       </c>
     </row>
     <row r="28" spans="2:16" s="1" customFormat="1" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="29"/>
+      <c r="B28" s="31"/>
       <c r="C28" s="24">
         <v>5</v>
       </c>
       <c r="D28" s="20">
         <v>7.5617000000000001</v>
       </c>
-      <c r="F28" s="29"/>
+      <c r="F28" s="31"/>
       <c r="G28" s="24">
         <v>5</v>
       </c>
       <c r="H28" s="20">
         <v>24.2681</v>
       </c>
-      <c r="J28" s="29"/>
+      <c r="J28" s="31"/>
       <c r="K28" s="24">
         <v>5</v>
       </c>
       <c r="L28" s="20">
         <v>33.433500000000002</v>
       </c>
-      <c r="N28" s="29"/>
+      <c r="N28" s="31"/>
       <c r="O28" s="24">
         <v>5</v>
       </c>
@@ -1627,644 +2790,759 @@
       </c>
     </row>
     <row r="29" spans="2:16" s="1" customFormat="1" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="30" t="s">
+      <c r="B29" s="32" t="s">
         <v>12</v>
       </c>
-      <c r="C29" s="31"/>
+      <c r="C29" s="33"/>
       <c r="D29" s="21">
         <f>AVERAGE(D24:D28)</f>
         <v>7.6337600000000005</v>
       </c>
-      <c r="F29" s="30" t="s">
+      <c r="F29" s="32" t="s">
         <v>12</v>
       </c>
-      <c r="G29" s="31"/>
+      <c r="G29" s="33"/>
       <c r="H29" s="21">
         <f>AVERAGE(H24:H28)</f>
         <v>24.58466</v>
       </c>
-      <c r="J29" s="30" t="s">
+      <c r="J29" s="32" t="s">
         <v>12</v>
       </c>
-      <c r="K29" s="31"/>
+      <c r="K29" s="33"/>
       <c r="L29" s="21">
         <f>AVERAGE(L24:L28)</f>
         <v>33.474100000000007</v>
       </c>
-      <c r="N29" s="30" t="s">
+      <c r="N29" s="32" t="s">
         <v>12</v>
       </c>
-      <c r="O29" s="31"/>
+      <c r="O29" s="33"/>
       <c r="P29" s="21">
         <f>AVERAGE(P24:P28)</f>
         <v>85.974559999999997</v>
       </c>
     </row>
-    <row r="30" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="31" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B31" s="32" t="s">
+    <row r="30" spans="2:16" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B30" s="18"/>
+      <c r="C30" s="18"/>
+      <c r="D30" s="18"/>
+      <c r="F30" s="18"/>
+      <c r="G30" s="18"/>
+      <c r="H30" s="18"/>
+      <c r="J30" s="18"/>
+      <c r="K30" s="18"/>
+      <c r="L30" s="18"/>
+      <c r="N30" s="18"/>
+      <c r="O30" s="18"/>
+      <c r="P30" s="18"/>
+    </row>
+    <row r="31" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="32" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B32" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="C31" s="33"/>
-      <c r="D31" s="34"/>
-      <c r="F31" s="32" t="s">
+      <c r="C32" s="35"/>
+      <c r="D32" s="36"/>
+      <c r="F32" s="34" t="s">
         <v>14</v>
       </c>
-      <c r="G31" s="33"/>
-      <c r="H31" s="34"/>
-      <c r="J31" s="32" t="s">
+      <c r="G32" s="35"/>
+      <c r="H32" s="36"/>
+      <c r="J32" s="34" t="s">
         <v>15</v>
       </c>
-      <c r="K31" s="33"/>
-      <c r="L31" s="34"/>
-      <c r="M31" s="1"/>
-      <c r="N31" s="32" t="s">
+      <c r="K32" s="35"/>
+      <c r="L32" s="36"/>
+      <c r="M32" s="1"/>
+      <c r="N32" s="34" t="s">
         <v>16</v>
       </c>
-      <c r="O31" s="33"/>
-      <c r="P31" s="34"/>
-    </row>
-    <row r="32" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B32" s="35"/>
-      <c r="C32" s="36"/>
-      <c r="D32" s="37"/>
-      <c r="F32" s="35"/>
-      <c r="G32" s="36"/>
-      <c r="H32" s="37"/>
-      <c r="J32" s="35"/>
-      <c r="K32" s="36"/>
-      <c r="L32" s="37"/>
-      <c r="M32" s="1"/>
-      <c r="N32" s="35"/>
-      <c r="O32" s="36"/>
-      <c r="P32" s="37"/>
-    </row>
-    <row r="33" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B33" s="28" t="s">
+      <c r="O32" s="35"/>
+      <c r="P32" s="36"/>
+    </row>
+    <row r="33" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B33" s="37"/>
+      <c r="C33" s="38"/>
+      <c r="D33" s="39"/>
+      <c r="F33" s="37"/>
+      <c r="G33" s="38"/>
+      <c r="H33" s="39"/>
+      <c r="J33" s="37"/>
+      <c r="K33" s="38"/>
+      <c r="L33" s="39"/>
+      <c r="M33" s="1"/>
+      <c r="N33" s="37"/>
+      <c r="O33" s="38"/>
+      <c r="P33" s="39"/>
+    </row>
+    <row r="34" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B34" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="C33" s="23">
+      <c r="C34" s="23">
         <v>1</v>
       </c>
-      <c r="D33" s="17">
+      <c r="D34" s="17">
         <v>15.8832</v>
       </c>
-      <c r="F33" s="28" t="s">
+      <c r="F34" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="G33" s="23">
+      <c r="G34" s="23">
         <v>1</v>
       </c>
-      <c r="H33" s="17">
+      <c r="H34" s="17">
         <v>16.741099999999999</v>
       </c>
-      <c r="J33" s="28" t="s">
+      <c r="J34" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="K33" s="23">
+      <c r="K34" s="23">
         <v>1</v>
       </c>
-      <c r="L33" s="17"/>
-      <c r="M33" s="1"/>
-      <c r="N33" s="28" t="s">
+      <c r="L34" s="28">
+        <v>16.8765</v>
+      </c>
+      <c r="M34" s="1"/>
+      <c r="N34" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="O33" s="23">
+      <c r="O34" s="23">
         <v>1</v>
       </c>
-      <c r="P33" s="17"/>
-    </row>
-    <row r="34" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B34" s="29"/>
-      <c r="C34" s="24">
+      <c r="P34" s="28">
+        <v>19.5139</v>
+      </c>
+    </row>
+    <row r="35" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B35" s="31"/>
+      <c r="C35" s="24">
         <v>2</v>
       </c>
-      <c r="D34" s="19">
+      <c r="D35" s="19">
         <v>15.7499</v>
       </c>
-      <c r="F34" s="29"/>
-      <c r="G34" s="24">
+      <c r="F35" s="31"/>
+      <c r="G35" s="24">
         <v>2</v>
       </c>
-      <c r="H34" s="19">
+      <c r="H35" s="19">
         <v>16.998200000000001</v>
       </c>
-      <c r="J34" s="29"/>
-      <c r="K34" s="24">
+      <c r="J35" s="31"/>
+      <c r="K35" s="24">
         <v>2</v>
       </c>
-      <c r="L34" s="19"/>
-      <c r="M34" s="1"/>
-      <c r="N34" s="29"/>
-      <c r="O34" s="24">
+      <c r="L35" s="19">
+        <v>16.7712</v>
+      </c>
+      <c r="M35" s="1"/>
+      <c r="N35" s="31"/>
+      <c r="O35" s="24">
         <v>2</v>
       </c>
-      <c r="P34" s="19"/>
-    </row>
-    <row r="35" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B35" s="29"/>
-      <c r="C35" s="24">
+      <c r="P35" s="19">
+        <v>21.908100000000001</v>
+      </c>
+    </row>
+    <row r="36" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B36" s="31"/>
+      <c r="C36" s="24">
         <v>3</v>
       </c>
-      <c r="D35" s="19">
+      <c r="D36" s="19">
         <v>15.984999999999999</v>
       </c>
-      <c r="F35" s="29"/>
-      <c r="G35" s="24">
+      <c r="F36" s="31"/>
+      <c r="G36" s="24">
         <v>3</v>
       </c>
-      <c r="H35" s="19">
+      <c r="H36" s="19">
         <v>17.138100000000001</v>
       </c>
-      <c r="J35" s="29"/>
-      <c r="K35" s="24">
+      <c r="J36" s="31"/>
+      <c r="K36" s="24">
         <v>3</v>
       </c>
-      <c r="L35" s="19"/>
-      <c r="M35" s="1"/>
-      <c r="N35" s="29"/>
-      <c r="O35" s="24">
+      <c r="L36" s="19">
+        <v>16.081700000000001</v>
+      </c>
+      <c r="M36" s="1"/>
+      <c r="N36" s="31"/>
+      <c r="O36" s="24">
         <v>3</v>
       </c>
-      <c r="P35" s="19"/>
-    </row>
-    <row r="36" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B36" s="29"/>
-      <c r="C36" s="24">
+      <c r="P36" s="19">
+        <v>20.832100000000001</v>
+      </c>
+    </row>
+    <row r="37" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B37" s="31"/>
+      <c r="C37" s="24">
         <v>4</v>
       </c>
-      <c r="D36" s="19">
+      <c r="D37" s="19">
         <v>15.6934</v>
       </c>
-      <c r="F36" s="29"/>
-      <c r="G36" s="24">
+      <c r="F37" s="31"/>
+      <c r="G37" s="24">
         <v>4</v>
       </c>
-      <c r="H36" s="19">
+      <c r="H37" s="19">
         <v>17.102399999999999</v>
       </c>
-      <c r="J36" s="29"/>
-      <c r="K36" s="24">
+      <c r="J37" s="31"/>
+      <c r="K37" s="24">
         <v>4</v>
       </c>
-      <c r="L36" s="19"/>
-      <c r="M36" s="1"/>
-      <c r="N36" s="29"/>
-      <c r="O36" s="24">
+      <c r="L37" s="19">
+        <v>16.82</v>
+      </c>
+      <c r="M37" s="1"/>
+      <c r="N37" s="31"/>
+      <c r="O37" s="24">
         <v>4</v>
       </c>
-      <c r="P36" s="19"/>
-    </row>
-    <row r="37" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B37" s="29"/>
-      <c r="C37" s="24">
+      <c r="P37" s="19">
+        <v>19.800599999999999</v>
+      </c>
+    </row>
+    <row r="38" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B38" s="31"/>
+      <c r="C38" s="24">
         <v>5</v>
       </c>
-      <c r="D37" s="20">
+      <c r="D38" s="20">
         <v>16.6691</v>
       </c>
-      <c r="F37" s="29"/>
-      <c r="G37" s="24">
+      <c r="F38" s="31"/>
+      <c r="G38" s="24">
         <v>5</v>
       </c>
-      <c r="H37" s="20">
+      <c r="H38" s="20">
         <v>16.9376</v>
       </c>
-      <c r="J37" s="29"/>
-      <c r="K37" s="24">
+      <c r="J38" s="31"/>
+      <c r="K38" s="24">
         <v>5</v>
       </c>
-      <c r="L37" s="20"/>
-      <c r="M37" s="1"/>
-      <c r="N37" s="29"/>
-      <c r="O37" s="24">
+      <c r="L38" s="29">
+        <v>16.113199999999999</v>
+      </c>
+      <c r="M38" s="1"/>
+      <c r="N38" s="31"/>
+      <c r="O38" s="24">
         <v>5</v>
       </c>
-      <c r="P37" s="20"/>
-    </row>
-    <row r="38" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B38" s="30" t="s">
+      <c r="P38" s="29">
+        <v>20.067499999999999</v>
+      </c>
+    </row>
+    <row r="39" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B39" s="32" t="s">
         <v>12</v>
       </c>
-      <c r="C38" s="31"/>
-      <c r="D38" s="21">
-        <f>AVERAGE(D33:D37)</f>
+      <c r="C39" s="33"/>
+      <c r="D39" s="21">
+        <f>AVERAGE(D34:D38)</f>
         <v>15.996119999999999</v>
       </c>
-      <c r="F38" s="30" t="s">
+      <c r="F39" s="32" t="s">
         <v>12</v>
       </c>
-      <c r="G38" s="31"/>
-      <c r="H38" s="21">
-        <f>AVERAGE(H33:H37)</f>
+      <c r="G39" s="33"/>
+      <c r="H39" s="21">
+        <f>AVERAGE(H34:H38)</f>
         <v>16.98348</v>
       </c>
-      <c r="J38" s="30" t="s">
+      <c r="J39" s="32" t="s">
         <v>12</v>
       </c>
-      <c r="K38" s="31"/>
-      <c r="L38" s="21" t="e">
-        <f>AVERAGE(L33:L37)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M38" s="1"/>
-      <c r="N38" s="30" t="s">
+      <c r="K39" s="33"/>
+      <c r="L39" s="21">
+        <f>AVERAGE(L34:L38)</f>
+        <v>16.532519999999998</v>
+      </c>
+      <c r="M39" s="1"/>
+      <c r="N39" s="32" t="s">
         <v>12</v>
       </c>
-      <c r="O38" s="31"/>
-      <c r="P38" s="21" t="e">
-        <f>AVERAGE(P33:P37)</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="39" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B39" s="22"/>
-      <c r="C39" s="18"/>
-      <c r="D39" s="19"/>
-      <c r="F39" s="22"/>
-      <c r="G39" s="18"/>
-      <c r="H39" s="19"/>
-      <c r="J39" s="22"/>
-      <c r="K39" s="18"/>
-      <c r="L39" s="19"/>
-      <c r="M39" s="1"/>
-      <c r="N39" s="22"/>
-      <c r="O39" s="18"/>
-      <c r="P39" s="19"/>
-    </row>
-    <row r="40" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B40" s="28" t="s">
+      <c r="O39" s="33"/>
+      <c r="P39" s="21">
+        <f>AVERAGE(P34:P38)</f>
+        <v>20.424439999999997</v>
+      </c>
+    </row>
+    <row r="40" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B40" s="22"/>
+      <c r="C40" s="18"/>
+      <c r="D40" s="19"/>
+      <c r="F40" s="22"/>
+      <c r="G40" s="18"/>
+      <c r="H40" s="19"/>
+      <c r="J40" s="22"/>
+      <c r="K40" s="18"/>
+      <c r="L40" s="19"/>
+      <c r="M40" s="1"/>
+      <c r="N40" s="22"/>
+      <c r="O40" s="18"/>
+      <c r="P40" s="19"/>
+    </row>
+    <row r="41" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B41" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="C40" s="23">
+      <c r="C41" s="23">
         <v>1</v>
       </c>
-      <c r="D40" s="17">
+      <c r="D41" s="17">
         <v>1149.1199999999999</v>
       </c>
-      <c r="F40" s="28" t="s">
+      <c r="F41" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="G40" s="23">
+      <c r="G41" s="23">
         <v>1</v>
       </c>
-      <c r="H40" s="17">
+      <c r="H41" s="17">
         <v>1724.41</v>
       </c>
-      <c r="J40" s="28" t="s">
+      <c r="J41" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="K40" s="23">
+      <c r="K41" s="23">
         <v>1</v>
       </c>
-      <c r="L40" s="17"/>
-      <c r="M40" s="1"/>
-      <c r="N40" s="28" t="s">
+      <c r="L41" s="28">
+        <v>2452.37</v>
+      </c>
+      <c r="M41" s="1"/>
+      <c r="N41" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="O40" s="23">
+      <c r="O41" s="23">
         <v>1</v>
       </c>
-      <c r="P40" s="17"/>
-    </row>
-    <row r="41" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B41" s="29"/>
-      <c r="C41" s="24">
+      <c r="P41" s="28">
+        <v>3303.74</v>
+      </c>
+    </row>
+    <row r="42" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B42" s="31"/>
+      <c r="C42" s="24">
         <v>2</v>
       </c>
-      <c r="D41" s="19">
+      <c r="D42" s="19">
         <v>1135.3900000000001</v>
       </c>
-      <c r="F41" s="29"/>
-      <c r="G41" s="24">
+      <c r="F42" s="31"/>
+      <c r="G42" s="24">
         <v>2</v>
       </c>
-      <c r="H41" s="19">
+      <c r="H42" s="19">
         <v>1740.63</v>
       </c>
-      <c r="J41" s="29"/>
-      <c r="K41" s="24">
+      <c r="J42" s="31"/>
+      <c r="K42" s="24">
         <v>2</v>
       </c>
-      <c r="L41" s="19"/>
-      <c r="M41" s="1"/>
-      <c r="N41" s="29"/>
-      <c r="O41" s="24">
+      <c r="L42" s="19">
+        <v>2467.63</v>
+      </c>
+      <c r="M42" s="1"/>
+      <c r="N42" s="31"/>
+      <c r="O42" s="24">
         <v>2</v>
       </c>
-      <c r="P41" s="19"/>
-    </row>
-    <row r="42" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B42" s="29"/>
-      <c r="C42" s="24">
+      <c r="P42" s="19">
+        <v>3314.94</v>
+      </c>
+    </row>
+    <row r="43" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B43" s="31"/>
+      <c r="C43" s="24">
         <v>3</v>
       </c>
-      <c r="D42" s="19">
+      <c r="D43" s="19">
         <v>1144.76</v>
       </c>
-      <c r="F42" s="29"/>
-      <c r="G42" s="24">
+      <c r="F43" s="31"/>
+      <c r="G43" s="24">
         <v>3</v>
       </c>
-      <c r="H42" s="19">
+      <c r="H43" s="19">
         <v>1734.38</v>
       </c>
-      <c r="J42" s="29"/>
-      <c r="K42" s="24">
+      <c r="J43" s="31"/>
+      <c r="K43" s="24">
         <v>3</v>
       </c>
-      <c r="L42" s="19"/>
-      <c r="M42" s="1"/>
-      <c r="N42" s="29"/>
-      <c r="O42" s="24">
+      <c r="L43" s="19">
+        <v>2451.73</v>
+      </c>
+      <c r="M43" s="1"/>
+      <c r="N43" s="31"/>
+      <c r="O43" s="24">
         <v>3</v>
       </c>
-      <c r="P42" s="19"/>
-    </row>
-    <row r="43" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B43" s="29"/>
-      <c r="C43" s="24">
+      <c r="P43" s="19">
+        <v>3311.8</v>
+      </c>
+    </row>
+    <row r="44" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B44" s="31"/>
+      <c r="C44" s="24">
         <v>4</v>
       </c>
-      <c r="D43" s="19">
+      <c r="D44" s="19">
         <v>1130.6500000000001</v>
       </c>
-      <c r="F43" s="29"/>
-      <c r="G43" s="24">
+      <c r="F44" s="31"/>
+      <c r="G44" s="24">
         <v>4</v>
       </c>
-      <c r="H43" s="19">
+      <c r="H44" s="19">
         <v>1757.13</v>
       </c>
-      <c r="J43" s="29"/>
-      <c r="K43" s="24">
+      <c r="J44" s="31"/>
+      <c r="K44" s="24">
         <v>4</v>
       </c>
-      <c r="L43" s="19"/>
-      <c r="M43" s="1"/>
-      <c r="N43" s="29"/>
-      <c r="O43" s="24">
+      <c r="L44" s="19">
+        <v>2460.17</v>
+      </c>
+      <c r="M44" s="1"/>
+      <c r="N44" s="31"/>
+      <c r="O44" s="24">
         <v>4</v>
       </c>
-      <c r="P43" s="19"/>
-    </row>
-    <row r="44" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B44" s="29"/>
-      <c r="C44" s="24">
+      <c r="P44" s="19">
+        <v>3320.34</v>
+      </c>
+    </row>
+    <row r="45" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B45" s="31"/>
+      <c r="C45" s="24">
         <v>5</v>
       </c>
-      <c r="D44" s="20">
+      <c r="D45" s="20">
         <v>1130.4100000000001</v>
       </c>
-      <c r="F44" s="29"/>
-      <c r="G44" s="24">
+      <c r="F45" s="31"/>
+      <c r="G45" s="24">
         <v>5</v>
       </c>
-      <c r="H44" s="20">
+      <c r="H45" s="20">
         <v>1741.6</v>
       </c>
-      <c r="J44" s="29"/>
-      <c r="K44" s="24">
+      <c r="J45" s="31"/>
+      <c r="K45" s="24">
         <v>5</v>
       </c>
-      <c r="L44" s="20"/>
-      <c r="M44" s="1"/>
-      <c r="N44" s="29"/>
-      <c r="O44" s="24">
+      <c r="L45" s="29">
+        <v>2443.19</v>
+      </c>
+      <c r="M45" s="1"/>
+      <c r="N45" s="31"/>
+      <c r="O45" s="24">
         <v>5</v>
       </c>
-      <c r="P44" s="20"/>
-    </row>
-    <row r="45" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B45" s="30" t="s">
+      <c r="P45" s="29">
+        <v>3292.1</v>
+      </c>
+    </row>
+    <row r="46" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B46" s="32" t="s">
         <v>12</v>
       </c>
-      <c r="C45" s="31"/>
-      <c r="D45" s="21">
-        <f>AVERAGE(D40:D44)</f>
+      <c r="C46" s="33"/>
+      <c r="D46" s="21">
+        <f>AVERAGE(D41:D45)</f>
         <v>1138.066</v>
       </c>
-      <c r="F45" s="30" t="s">
+      <c r="F46" s="32" t="s">
         <v>12</v>
       </c>
-      <c r="G45" s="31"/>
-      <c r="H45" s="21">
-        <f>AVERAGE(H40:H44)</f>
+      <c r="G46" s="33"/>
+      <c r="H46" s="21">
+        <f>AVERAGE(H41:H45)</f>
         <v>1739.6299999999999</v>
       </c>
-      <c r="J45" s="30" t="s">
+      <c r="J46" s="32" t="s">
         <v>12</v>
       </c>
-      <c r="K45" s="31"/>
-      <c r="L45" s="21" t="e">
-        <f>AVERAGE(L40:L44)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M45" s="1"/>
-      <c r="N45" s="30" t="s">
+      <c r="K46" s="33"/>
+      <c r="L46" s="21">
+        <f>AVERAGE(L41:L45)</f>
+        <v>2455.018</v>
+      </c>
+      <c r="M46" s="1"/>
+      <c r="N46" s="32" t="s">
         <v>12</v>
       </c>
-      <c r="O45" s="31"/>
-      <c r="P45" s="21" t="e">
-        <f>AVERAGE(P40:P44)</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="46" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B46" s="22"/>
-      <c r="C46" s="18"/>
-      <c r="D46" s="19"/>
-      <c r="F46" s="22"/>
-      <c r="G46" s="18"/>
-      <c r="H46" s="19"/>
-      <c r="J46" s="22"/>
-      <c r="K46" s="18"/>
-      <c r="L46" s="19"/>
-      <c r="M46" s="1"/>
-      <c r="N46" s="22"/>
-      <c r="O46" s="18"/>
-      <c r="P46" s="19"/>
-    </row>
-    <row r="47" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B47" s="28" t="s">
+      <c r="O46" s="33"/>
+      <c r="P46" s="21">
+        <f>AVERAGE(P41:P45)</f>
+        <v>3308.5839999999998</v>
+      </c>
+    </row>
+    <row r="47" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B47" s="22"/>
+      <c r="C47" s="18"/>
+      <c r="D47" s="19"/>
+      <c r="F47" s="22"/>
+      <c r="G47" s="18"/>
+      <c r="H47" s="19"/>
+      <c r="J47" s="22"/>
+      <c r="K47" s="18"/>
+      <c r="L47" s="19"/>
+      <c r="M47" s="1"/>
+      <c r="N47" s="22"/>
+      <c r="O47" s="18"/>
+      <c r="P47" s="19"/>
+    </row>
+    <row r="48" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B48" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="C47" s="23">
+      <c r="C48" s="23">
         <v>1</v>
       </c>
-      <c r="D47" s="17">
+      <c r="D48" s="17">
         <v>107.738</v>
       </c>
-      <c r="F47" s="28" t="s">
+      <c r="F48" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="G47" s="23">
+      <c r="G48" s="23">
         <v>1</v>
       </c>
-      <c r="H47" s="17">
+      <c r="H48" s="17">
         <v>120.848</v>
       </c>
-      <c r="J47" s="28" t="s">
+      <c r="J48" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="K47" s="23">
+      <c r="K48" s="23">
         <v>1</v>
       </c>
-      <c r="L47" s="17"/>
-      <c r="M47" s="1"/>
-      <c r="N47" s="28" t="s">
+      <c r="L48" s="28">
+        <v>424.72399999999999</v>
+      </c>
+      <c r="M48" s="1"/>
+      <c r="N48" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="O47" s="23">
+      <c r="O48" s="23">
         <v>1</v>
       </c>
-      <c r="P47" s="17"/>
-    </row>
-    <row r="48" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B48" s="29"/>
-      <c r="C48" s="24">
+      <c r="P48" s="28">
+        <v>425.327</v>
+      </c>
+    </row>
+    <row r="49" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B49" s="31"/>
+      <c r="C49" s="24">
         <v>2</v>
       </c>
-      <c r="D48" s="19">
+      <c r="D49" s="19">
         <v>105.935</v>
       </c>
-      <c r="F48" s="29"/>
-      <c r="G48" s="24">
+      <c r="F49" s="31"/>
+      <c r="G49" s="24">
         <v>2</v>
       </c>
-      <c r="H48" s="19">
+      <c r="H49" s="19">
         <v>118.76900000000001</v>
       </c>
-      <c r="J48" s="29"/>
-      <c r="K48" s="24">
+      <c r="J49" s="31"/>
+      <c r="K49" s="24">
         <v>2</v>
       </c>
-      <c r="L48" s="19"/>
-      <c r="M48" s="1"/>
-      <c r="N48" s="29"/>
-      <c r="O48" s="24">
+      <c r="L49" s="19">
+        <v>424.33300000000003</v>
+      </c>
+      <c r="M49" s="1"/>
+      <c r="N49" s="31"/>
+      <c r="O49" s="24">
         <v>2</v>
       </c>
-      <c r="P48" s="19"/>
-    </row>
-    <row r="49" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B49" s="29"/>
-      <c r="C49" s="24">
+      <c r="P49" s="19">
+        <v>426.33199999999999</v>
+      </c>
+    </row>
+    <row r="50" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B50" s="31"/>
+      <c r="C50" s="24">
         <v>3</v>
       </c>
-      <c r="D49" s="19">
+      <c r="D50" s="19">
         <v>106.126</v>
       </c>
-      <c r="F49" s="29"/>
-      <c r="G49" s="24">
+      <c r="F50" s="31"/>
+      <c r="G50" s="24">
         <v>3</v>
       </c>
-      <c r="H49" s="19">
+      <c r="H50" s="19">
         <v>119.114</v>
       </c>
-      <c r="J49" s="29"/>
-      <c r="K49" s="24">
+      <c r="J50" s="31"/>
+      <c r="K50" s="24">
         <v>3</v>
       </c>
-      <c r="L49" s="19"/>
-      <c r="M49" s="1"/>
-      <c r="N49" s="29"/>
-      <c r="O49" s="24">
+      <c r="L50" s="19">
+        <v>425.11599999999999</v>
+      </c>
+      <c r="M50" s="1"/>
+      <c r="N50" s="31"/>
+      <c r="O50" s="24">
         <v>3</v>
       </c>
-      <c r="P49" s="19"/>
-    </row>
-    <row r="50" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B50" s="29"/>
-      <c r="C50" s="24">
+      <c r="P50" s="19">
+        <v>423.73</v>
+      </c>
+    </row>
+    <row r="51" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B51" s="31"/>
+      <c r="C51" s="24">
         <v>4</v>
       </c>
-      <c r="D50" s="19">
+      <c r="D51" s="19">
         <v>105.5</v>
       </c>
-      <c r="F50" s="29"/>
-      <c r="G50" s="24">
+      <c r="F51" s="31"/>
+      <c r="G51" s="24">
         <v>4</v>
       </c>
-      <c r="H50" s="19">
+      <c r="H51" s="19">
         <v>121.352</v>
       </c>
-      <c r="J50" s="29"/>
-      <c r="K50" s="24">
+      <c r="J51" s="31"/>
+      <c r="K51" s="24">
         <v>4</v>
       </c>
-      <c r="L50" s="19"/>
-      <c r="M50" s="1"/>
-      <c r="N50" s="29"/>
-      <c r="O50" s="24">
+      <c r="L51" s="19">
+        <v>422.06</v>
+      </c>
+      <c r="M51" s="1"/>
+      <c r="N51" s="31"/>
+      <c r="O51" s="24">
         <v>4</v>
       </c>
-      <c r="P50" s="19"/>
-    </row>
-    <row r="51" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B51" s="29"/>
-      <c r="C51" s="24">
+      <c r="P51" s="19">
+        <v>424.80399999999997</v>
+      </c>
+    </row>
+    <row r="52" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B52" s="31"/>
+      <c r="C52" s="24">
         <v>5</v>
       </c>
-      <c r="D51" s="20">
+      <c r="D52" s="20">
         <v>106.129</v>
       </c>
-      <c r="F51" s="29"/>
-      <c r="G51" s="24">
+      <c r="F52" s="31"/>
+      <c r="G52" s="24">
         <v>5</v>
       </c>
-      <c r="H51" s="20">
+      <c r="H52" s="20">
         <v>118.878</v>
       </c>
-      <c r="J51" s="29"/>
-      <c r="K51" s="24">
+      <c r="J52" s="31"/>
+      <c r="K52" s="24">
         <v>5</v>
       </c>
-      <c r="L51" s="20"/>
-      <c r="M51" s="1"/>
-      <c r="N51" s="29"/>
-      <c r="O51" s="24">
+      <c r="L52" s="29">
+        <v>429.78899999999999</v>
+      </c>
+      <c r="M52" s="1"/>
+      <c r="N52" s="31"/>
+      <c r="O52" s="24">
         <v>5</v>
       </c>
-      <c r="P51" s="20"/>
-    </row>
-    <row r="52" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B52" s="30" t="s">
+      <c r="P52" s="29">
+        <v>435.17099999999999</v>
+      </c>
+    </row>
+    <row r="53" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B53" s="32" t="s">
         <v>12</v>
       </c>
-      <c r="C52" s="31"/>
-      <c r="D52" s="21">
-        <f>AVERAGE(D47:D51)</f>
+      <c r="C53" s="33"/>
+      <c r="D53" s="21">
+        <f>AVERAGE(D48:D52)</f>
         <v>106.2856</v>
       </c>
-      <c r="F52" s="30" t="s">
+      <c r="F53" s="32" t="s">
         <v>12</v>
       </c>
-      <c r="G52" s="31"/>
-      <c r="H52" s="21">
-        <f>AVERAGE(H47:H51)</f>
+      <c r="G53" s="33"/>
+      <c r="H53" s="21">
+        <f>AVERAGE(H48:H52)</f>
         <v>119.79220000000001</v>
       </c>
-      <c r="J52" s="30" t="s">
+      <c r="J53" s="32" t="s">
         <v>12</v>
       </c>
-      <c r="K52" s="31"/>
-      <c r="L52" s="21" t="e">
-        <f>AVERAGE(L47:L51)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M52" s="1"/>
-      <c r="N52" s="30" t="s">
+      <c r="K53" s="33"/>
+      <c r="L53" s="21">
+        <f>AVERAGE(L48:L52)</f>
+        <v>425.20439999999996</v>
+      </c>
+      <c r="M53" s="1"/>
+      <c r="N53" s="32" t="s">
         <v>12</v>
       </c>
-      <c r="O52" s="31"/>
-      <c r="P52" s="21" t="e">
-        <f>AVERAGE(P47:P51)</f>
-        <v>#DIV/0!</v>
+      <c r="O53" s="33"/>
+      <c r="P53" s="21">
+        <f>AVERAGE(P48:P52)</f>
+        <v>427.07280000000003</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="57">
+    <mergeCell ref="B48:B52"/>
+    <mergeCell ref="F48:F52"/>
+    <mergeCell ref="J48:J52"/>
+    <mergeCell ref="N48:N52"/>
+    <mergeCell ref="B53:C53"/>
+    <mergeCell ref="F53:G53"/>
+    <mergeCell ref="J53:K53"/>
+    <mergeCell ref="N53:O53"/>
+    <mergeCell ref="B41:B45"/>
+    <mergeCell ref="F41:F45"/>
+    <mergeCell ref="J41:J45"/>
+    <mergeCell ref="N41:N45"/>
+    <mergeCell ref="B46:C46"/>
+    <mergeCell ref="F46:G46"/>
+    <mergeCell ref="J46:K46"/>
+    <mergeCell ref="N46:O46"/>
+    <mergeCell ref="B34:B38"/>
+    <mergeCell ref="F34:F38"/>
+    <mergeCell ref="J34:J38"/>
+    <mergeCell ref="N34:N38"/>
+    <mergeCell ref="B39:C39"/>
+    <mergeCell ref="F39:G39"/>
+    <mergeCell ref="J39:K39"/>
+    <mergeCell ref="N39:O39"/>
+    <mergeCell ref="N29:O29"/>
+    <mergeCell ref="B32:D33"/>
+    <mergeCell ref="F32:H33"/>
+    <mergeCell ref="J32:L33"/>
+    <mergeCell ref="N32:P33"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="F15:G15"/>
+    <mergeCell ref="F22:G22"/>
+    <mergeCell ref="F29:G29"/>
+    <mergeCell ref="J15:K15"/>
+    <mergeCell ref="J22:K22"/>
+    <mergeCell ref="J29:K29"/>
+    <mergeCell ref="C2:K2"/>
+    <mergeCell ref="B8:D9"/>
+    <mergeCell ref="F8:H9"/>
+    <mergeCell ref="J8:L9"/>
+    <mergeCell ref="N8:P9"/>
     <mergeCell ref="B24:B28"/>
     <mergeCell ref="F24:F28"/>
     <mergeCell ref="J24:J28"/>
@@ -2281,49 +3559,9 @@
     <mergeCell ref="B22:C22"/>
     <mergeCell ref="N15:O15"/>
     <mergeCell ref="N22:O22"/>
-    <mergeCell ref="C2:K2"/>
-    <mergeCell ref="B8:D9"/>
-    <mergeCell ref="F8:H9"/>
-    <mergeCell ref="J8:L9"/>
-    <mergeCell ref="N8:P9"/>
-    <mergeCell ref="F15:G15"/>
-    <mergeCell ref="F22:G22"/>
-    <mergeCell ref="F29:G29"/>
-    <mergeCell ref="J15:K15"/>
-    <mergeCell ref="J22:K22"/>
-    <mergeCell ref="J29:K29"/>
-    <mergeCell ref="N29:O29"/>
-    <mergeCell ref="B31:D32"/>
-    <mergeCell ref="F31:H32"/>
-    <mergeCell ref="J31:L32"/>
-    <mergeCell ref="N31:P32"/>
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="B33:B37"/>
-    <mergeCell ref="F33:F37"/>
-    <mergeCell ref="J33:J37"/>
-    <mergeCell ref="N33:N37"/>
-    <mergeCell ref="B38:C38"/>
-    <mergeCell ref="F38:G38"/>
-    <mergeCell ref="J38:K38"/>
-    <mergeCell ref="N38:O38"/>
-    <mergeCell ref="B40:B44"/>
-    <mergeCell ref="F40:F44"/>
-    <mergeCell ref="J40:J44"/>
-    <mergeCell ref="N40:N44"/>
-    <mergeCell ref="B45:C45"/>
-    <mergeCell ref="F45:G45"/>
-    <mergeCell ref="J45:K45"/>
-    <mergeCell ref="N45:O45"/>
-    <mergeCell ref="B47:B51"/>
-    <mergeCell ref="F47:F51"/>
-    <mergeCell ref="J47:J51"/>
-    <mergeCell ref="N47:N51"/>
-    <mergeCell ref="B52:C52"/>
-    <mergeCell ref="F52:G52"/>
-    <mergeCell ref="J52:K52"/>
-    <mergeCell ref="N52:O52"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Reuploaded files to repository
</commit_message>
<xml_diff>
--- a/z_HybridAlgorithmResults.xlsx
+++ b/z_HybridAlgorithmResults.xlsx
@@ -222,15 +222,6 @@
     <xf numFmtId="0" fontId="4" fillId="7" borderId="3" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="4" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="5" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="6" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -259,6 +250,15 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="4" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="5" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="6" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -302,10 +302,11 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" baseline="0">
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="lt1">
-                    <a:lumMod val="85000"/>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
@@ -334,10 +335,11 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" baseline="0">
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="lt1">
-                  <a:lumMod val="85000"/>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
                 </a:schemeClr>
               </a:solidFill>
               <a:latin typeface="+mn-lt"/>
@@ -374,37 +376,24 @@
               <a:solidFill>
                 <a:schemeClr val="accent1"/>
               </a:solidFill>
+              <a:round/>
             </a:ln>
-            <a:effectLst>
-              <a:glow rad="139700">
-                <a:schemeClr val="accent1">
-                  <a:satMod val="175000"/>
-                  <a:alpha val="14000"/>
-                </a:schemeClr>
-              </a:glow>
-            </a:effectLst>
+            <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="3"/>
+            <c:symbol val="diamond"/>
+            <c:size val="6"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent1">
-                  <a:lumMod val="60000"/>
-                  <a:lumOff val="40000"/>
-                </a:schemeClr>
+                <a:schemeClr val="accent1"/>
               </a:solidFill>
-              <a:ln>
-                <a:noFill/>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:round/>
               </a:ln>
-              <a:effectLst>
-                <a:glow rad="63500">
-                  <a:schemeClr val="accent1">
-                    <a:satMod val="175000"/>
-                    <a:alpha val="25000"/>
-                  </a:schemeClr>
-                </a:glow>
-              </a:effectLst>
+              <a:effectLst/>
             </c:spPr>
           </c:marker>
           <c:xVal>
@@ -566,37 +555,24 @@
               <a:solidFill>
                 <a:schemeClr val="accent2"/>
               </a:solidFill>
+              <a:round/>
             </a:ln>
-            <a:effectLst>
-              <a:glow rad="139700">
-                <a:schemeClr val="accent2">
-                  <a:satMod val="175000"/>
-                  <a:alpha val="14000"/>
-                </a:schemeClr>
-              </a:glow>
-            </a:effectLst>
+            <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="3"/>
+            <c:symbol val="square"/>
+            <c:size val="6"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent2">
-                  <a:lumMod val="60000"/>
-                  <a:lumOff val="40000"/>
-                </a:schemeClr>
+                <a:schemeClr val="accent2"/>
               </a:solidFill>
-              <a:ln>
-                <a:noFill/>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+                <a:round/>
               </a:ln>
-              <a:effectLst>
-                <a:glow rad="63500">
-                  <a:schemeClr val="accent2">
-                    <a:satMod val="175000"/>
-                    <a:alpha val="25000"/>
-                  </a:schemeClr>
-                </a:glow>
-              </a:effectLst>
+              <a:effectLst/>
             </c:spPr>
           </c:marker>
           <c:xVal>
@@ -744,11 +720,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2079581648"/>
-        <c:axId val="-2079583824"/>
+        <c:axId val="-257193040"/>
+        <c:axId val="-257190864"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2079581648"/>
+        <c:axId val="-257193040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -758,10 +734,9 @@
           <c:spPr>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
               <a:solidFill>
-                <a:schemeClr val="dk1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                  <a:alpha val="75000"/>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
                 </a:schemeClr>
               </a:solidFill>
               <a:round/>
@@ -776,10 +751,11 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="lt1">
-                        <a:lumMod val="75000"/>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
                       </a:schemeClr>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
@@ -808,10 +784,11 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
                   <a:solidFill>
-                    <a:schemeClr val="lt1">
-                      <a:lumMod val="75000"/>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
                     </a:schemeClr>
                   </a:solidFill>
                   <a:latin typeface="+mn-lt"/>
@@ -829,8 +806,14 @@
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
-          <a:ln>
-            <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="dk1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
           </a:ln>
           <a:effectLst/>
         </c:spPr>
@@ -841,8 +824,9 @@
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="lt1">
-                    <a:lumMod val="75000"/>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
@@ -853,12 +837,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2079583824"/>
+        <c:crossAx val="-257190864"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2079583824"/>
+        <c:axId val="-257190864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -868,10 +852,9 @@
           <c:spPr>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
               <a:solidFill>
-                <a:schemeClr val="dk1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                  <a:alpha val="75000"/>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
                 </a:schemeClr>
               </a:solidFill>
               <a:round/>
@@ -886,10 +869,11 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="lt1">
-                        <a:lumMod val="75000"/>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
                       </a:schemeClr>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
@@ -899,7 +883,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
-                  <a:t>Runtime in ms</a:t>
+                  <a:t>Average Runtime in ms</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -918,10 +902,11 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
                   <a:solidFill>
-                    <a:schemeClr val="lt1">
-                      <a:lumMod val="75000"/>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
                     </a:schemeClr>
                   </a:solidFill>
                   <a:latin typeface="+mn-lt"/>
@@ -941,8 +926,9 @@
           <a:noFill/>
           <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
-              <a:schemeClr val="lt1">
-                <a:lumMod val="50000"/>
+              <a:schemeClr val="dk1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
               </a:schemeClr>
             </a:solidFill>
             <a:round/>
@@ -956,8 +942,9 @@
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="lt1">
-                    <a:lumMod val="75000"/>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
@@ -968,7 +955,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2079581648"/>
+        <c:crossAx val="-257193040"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -998,8 +985,9 @@
           <a:pPr>
             <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="lt1">
-                  <a:lumMod val="75000"/>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
                 </a:schemeClr>
               </a:solidFill>
               <a:latin typeface="+mn-lt"/>
@@ -1017,14 +1005,11 @@
   </c:chart>
   <c:spPr>
     <a:solidFill>
-      <a:schemeClr val="dk1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
-      </a:schemeClr>
+      <a:schemeClr val="lt1"/>
     </a:solidFill>
     <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
       <a:solidFill>
-        <a:schemeClr val="dk1">
+        <a:schemeClr val="tx1">
           <a:lumMod val="15000"/>
           <a:lumOff val="85000"/>
         </a:schemeClr>
@@ -1072,10 +1057,11 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" baseline="0">
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="lt1">
-                    <a:lumMod val="85000"/>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
@@ -1104,10 +1090,11 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" baseline="0">
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="lt1">
-                  <a:lumMod val="85000"/>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
                 </a:schemeClr>
               </a:solidFill>
               <a:latin typeface="+mn-lt"/>
@@ -1144,37 +1131,24 @@
               <a:solidFill>
                 <a:schemeClr val="accent1"/>
               </a:solidFill>
+              <a:round/>
             </a:ln>
-            <a:effectLst>
-              <a:glow rad="139700">
-                <a:schemeClr val="accent1">
-                  <a:satMod val="175000"/>
-                  <a:alpha val="14000"/>
-                </a:schemeClr>
-              </a:glow>
-            </a:effectLst>
+            <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="3"/>
+            <c:symbol val="diamond"/>
+            <c:size val="6"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent1">
-                  <a:lumMod val="60000"/>
-                  <a:lumOff val="40000"/>
-                </a:schemeClr>
+                <a:schemeClr val="accent1"/>
               </a:solidFill>
-              <a:ln>
-                <a:noFill/>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:round/>
               </a:ln>
-              <a:effectLst>
-                <a:glow rad="63500">
-                  <a:schemeClr val="accent1">
-                    <a:satMod val="175000"/>
-                    <a:alpha val="25000"/>
-                  </a:schemeClr>
-                </a:glow>
-              </a:effectLst>
+              <a:effectLst/>
             </c:spPr>
           </c:marker>
           <c:xVal>
@@ -1336,37 +1310,24 @@
               <a:solidFill>
                 <a:schemeClr val="accent2"/>
               </a:solidFill>
+              <a:round/>
             </a:ln>
-            <a:effectLst>
-              <a:glow rad="139700">
-                <a:schemeClr val="accent2">
-                  <a:satMod val="175000"/>
-                  <a:alpha val="14000"/>
-                </a:schemeClr>
-              </a:glow>
-            </a:effectLst>
+            <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="3"/>
+            <c:symbol val="square"/>
+            <c:size val="6"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent2">
-                  <a:lumMod val="60000"/>
-                  <a:lumOff val="40000"/>
-                </a:schemeClr>
+                <a:schemeClr val="accent2"/>
               </a:solidFill>
-              <a:ln>
-                <a:noFill/>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+                <a:round/>
               </a:ln>
-              <a:effectLst>
-                <a:glow rad="63500">
-                  <a:schemeClr val="accent2">
-                    <a:satMod val="175000"/>
-                    <a:alpha val="25000"/>
-                  </a:schemeClr>
-                </a:glow>
-              </a:effectLst>
+              <a:effectLst/>
             </c:spPr>
           </c:marker>
           <c:xVal>
@@ -1517,11 +1478,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1990487904"/>
-        <c:axId val="-1990484640"/>
+        <c:axId val="-257189776"/>
+        <c:axId val="-257205008"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1990487904"/>
+        <c:axId val="-257189776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1531,10 +1492,9 @@
           <c:spPr>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
               <a:solidFill>
-                <a:schemeClr val="dk1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                  <a:alpha val="75000"/>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
                 </a:schemeClr>
               </a:solidFill>
               <a:round/>
@@ -1549,10 +1509,11 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="lt1">
-                        <a:lumMod val="75000"/>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
                       </a:schemeClr>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
@@ -1562,13 +1523,8 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
-                  <a:t>Number of Elements</a:t>
+                  <a:t>Number of Elements n</a:t>
                 </a:r>
-                <a:r>
-                  <a:rPr lang="en-US" baseline="0"/>
-                  <a:t> n</a:t>
-                </a:r>
-                <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:rich>
           </c:tx>
@@ -1586,10 +1542,11 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
                   <a:solidFill>
-                    <a:schemeClr val="lt1">
-                      <a:lumMod val="75000"/>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
                     </a:schemeClr>
                   </a:solidFill>
                   <a:latin typeface="+mn-lt"/>
@@ -1607,8 +1564,14 @@
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
-          <a:ln>
-            <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="dk1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
           </a:ln>
           <a:effectLst/>
         </c:spPr>
@@ -1619,8 +1582,9 @@
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="lt1">
-                    <a:lumMod val="75000"/>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
@@ -1631,12 +1595,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1990484640"/>
+        <c:crossAx val="-257205008"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1990484640"/>
+        <c:axId val="-257205008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1646,10 +1610,9 @@
           <c:spPr>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
               <a:solidFill>
-                <a:schemeClr val="dk1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                  <a:alpha val="75000"/>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
                 </a:schemeClr>
               </a:solidFill>
               <a:round/>
@@ -1664,10 +1627,11 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="lt1">
-                        <a:lumMod val="75000"/>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
                       </a:schemeClr>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
@@ -1677,7 +1641,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
-                  <a:t>Runtime in sm</a:t>
+                  <a:t>Average Runtime in sm</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -1696,10 +1660,11 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
                   <a:solidFill>
-                    <a:schemeClr val="lt1">
-                      <a:lumMod val="75000"/>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
                     </a:schemeClr>
                   </a:solidFill>
                   <a:latin typeface="+mn-lt"/>
@@ -1719,8 +1684,9 @@
           <a:noFill/>
           <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
-              <a:schemeClr val="lt1">
-                <a:lumMod val="50000"/>
+              <a:schemeClr val="dk1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
               </a:schemeClr>
             </a:solidFill>
             <a:round/>
@@ -1734,8 +1700,9 @@
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="lt1">
-                    <a:lumMod val="75000"/>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
@@ -1746,7 +1713,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1990487904"/>
+        <c:crossAx val="-257189776"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1776,8 +1743,9 @@
           <a:pPr>
             <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="lt1">
-                  <a:lumMod val="75000"/>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
                 </a:schemeClr>
               </a:solidFill>
               <a:latin typeface="+mn-lt"/>
@@ -1795,14 +1763,11 @@
   </c:chart>
   <c:spPr>
     <a:solidFill>
-      <a:schemeClr val="dk1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
-      </a:schemeClr>
+      <a:schemeClr val="lt1"/>
     </a:solidFill>
     <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
       <a:solidFill>
-        <a:schemeClr val="dk1">
+        <a:schemeClr val="tx1">
           <a:lumMod val="15000"/>
           <a:lumOff val="85000"/>
         </a:schemeClr>
@@ -1910,46 +1875,33 @@
 </file>
 
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="245">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="241">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="75000"/>
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="900" b="1" kern="1200"/>
+    <cs:defRPr sz="900" kern="1200" cap="all"/>
   </cs:axisTitle>
   <cs:categoryAxis>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="75000"/>
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="75000"/>
-          <a:lumOff val="25000"/>
-        </a:schemeClr>
-      </a:solidFill>
+    <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="dk1">
+          <a:schemeClr val="tx1">
             <a:lumMod val="15000"/>
             <a:lumOff val="85000"/>
           </a:schemeClr>
@@ -1957,6 +1909,29 @@
         <a:round/>
       </a:ln>
     </cs:spPr>
+    <cs:defRPr sz="900" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:chartArea>
   <cs:dataLabel>
@@ -1964,29 +1939,35 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="75000"/>
+      <a:schemeClr val="tx1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
+    <cs:defRPr sz="800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0"/>
   </cs:dataLabel>
   <cs:dataLabelCallout>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="15000"/>
-        <a:lumOff val="85000"/>
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="65000"/>
-          <a:lumOff val="35000"/>
-        </a:schemeClr>
+        <a:schemeClr val="lt1"/>
       </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
     </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
     <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
@@ -1994,73 +1975,41 @@
     </cs:bodyPr>
   </cs:dataLabelCallout>
   <cs:dataPoint>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:effectRef>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:miter lim="800000"/>
-      </a:ln>
-      <a:effectLst>
-        <a:glow rad="63500">
-          <a:schemeClr val="phClr">
-            <a:satMod val="175000"/>
-            <a:alpha val="25000"/>
-          </a:schemeClr>
-        </a:glow>
-      </a:effectLst>
-    </cs:spPr>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
+    <cs:lnRef idx="0"/>
     <cs:fillRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="0">
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
       <cs:styleClr val="auto"/>
-    </cs:effectRef>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:miter lim="800000"/>
-      </a:ln>
-      <a:effectLst>
-        <a:glow rad="63500">
-          <a:schemeClr val="phClr">
-            <a:satMod val="175000"/>
-            <a:alpha val="25000"/>
-          </a:schemeClr>
-        </a:glow>
-      </a:effectLst>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
     </cs:spPr>
   </cs:dataPoint3D>
   <cs:dataPointLine>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:effectRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="dk1"/>
     </cs:fontRef>
@@ -2069,15 +2018,8 @@
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
+        <a:round/>
       </a:ln>
-      <a:effectLst>
-        <a:glow rad="139700">
-          <a:schemeClr val="phClr">
-            <a:satMod val="175000"/>
-            <a:alpha val="14000"/>
-          </a:schemeClr>
-        </a:glow>
-      </a:effectLst>
     </cs:spPr>
   </cs:dataPointLine>
   <cs:dataPointMarker>
@@ -2087,30 +2029,23 @@
     <cs:fillRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:effectRef>
+    <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
-        <a:schemeClr val="phClr">
-          <a:lumMod val="60000"/>
-          <a:lumOff val="40000"/>
-        </a:schemeClr>
+        <a:schemeClr val="phClr"/>
       </a:solidFill>
-      <a:effectLst>
-        <a:glow rad="63500">
-          <a:schemeClr val="phClr">
-            <a:satMod val="175000"/>
-            <a:alpha val="25000"/>
-          </a:schemeClr>
-        </a:glow>
-      </a:effectLst>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
     </cs:spPr>
   </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="3"/>
+  <cs:dataPointMarkerLayout size="6"/>
   <cs:dataPointWireframe>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
@@ -2134,16 +2069,17 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="75000"/>
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
       </a:ln>
@@ -2151,327 +2087,6 @@
     <cs:defRPr sz="900" kern="1200"/>
   </cs:dataTable>
   <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="50000"/>
-          <a:lumOff val="50000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="50000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="50000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-            <a:alpha val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-            <a:alpha val="25000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="50000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="50000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="75000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="75000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="50000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="85000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1400" b="1" kern="1200" cap="none" baseline="0"/>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="25400" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:alpha val="50000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:trendline>
-  <cs:trendlineLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="75000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1">
-          <a:lumMod val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="50000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="75000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="50000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr/>
-  </cs:valueAxis>
-  <cs:wall>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-  </cs:wall>
-</cs:chartStyle>
-</file>
-
-<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="245">
-  <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="75000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" b="1" kern="1200"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="75000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
@@ -2485,6 +2100,277 @@
           <a:lumOff val="25000"/>
         </a:schemeClr>
       </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="800" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="dk1">
@@ -2496,35 +2382,112 @@
       </a:ln>
     </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="241">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200" cap="all"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
   </cs:chartArea>
   <cs:dataLabel>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="75000"/>
+      <a:schemeClr val="tx1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
+    <cs:defRPr sz="800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0"/>
   </cs:dataLabel>
   <cs:dataLabelCallout>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="15000"/>
-        <a:lumOff val="85000"/>
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="65000"/>
-          <a:lumOff val="35000"/>
-        </a:schemeClr>
+        <a:schemeClr val="lt1"/>
       </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
     </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
     <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
@@ -2532,73 +2495,41 @@
     </cs:bodyPr>
   </cs:dataLabelCallout>
   <cs:dataPoint>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:effectRef>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:miter lim="800000"/>
-      </a:ln>
-      <a:effectLst>
-        <a:glow rad="63500">
-          <a:schemeClr val="phClr">
-            <a:satMod val="175000"/>
-            <a:alpha val="25000"/>
-          </a:schemeClr>
-        </a:glow>
-      </a:effectLst>
-    </cs:spPr>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
+    <cs:lnRef idx="0"/>
     <cs:fillRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="0">
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
       <cs:styleClr val="auto"/>
-    </cs:effectRef>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:miter lim="800000"/>
-      </a:ln>
-      <a:effectLst>
-        <a:glow rad="63500">
-          <a:schemeClr val="phClr">
-            <a:satMod val="175000"/>
-            <a:alpha val="25000"/>
-          </a:schemeClr>
-        </a:glow>
-      </a:effectLst>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
     </cs:spPr>
   </cs:dataPoint3D>
   <cs:dataPointLine>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:effectRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="dk1"/>
     </cs:fontRef>
@@ -2607,15 +2538,8 @@
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
+        <a:round/>
       </a:ln>
-      <a:effectLst>
-        <a:glow rad="139700">
-          <a:schemeClr val="phClr">
-            <a:satMod val="175000"/>
-            <a:alpha val="14000"/>
-          </a:schemeClr>
-        </a:glow>
-      </a:effectLst>
     </cs:spPr>
   </cs:dataPointLine>
   <cs:dataPointMarker>
@@ -2625,30 +2549,23 @@
     <cs:fillRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:effectRef>
+    <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
-        <a:schemeClr val="phClr">
-          <a:lumMod val="60000"/>
-          <a:lumOff val="40000"/>
-        </a:schemeClr>
+        <a:schemeClr val="phClr"/>
       </a:solidFill>
-      <a:effectLst>
-        <a:glow rad="63500">
-          <a:schemeClr val="phClr">
-            <a:satMod val="175000"/>
-            <a:alpha val="25000"/>
-          </a:schemeClr>
-        </a:glow>
-      </a:effectLst>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
     </cs:spPr>
   </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="3"/>
+  <cs:dataPointMarkerLayout size="6"/>
   <cs:dataPointWireframe>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
@@ -2672,16 +2589,17 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="75000"/>
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
       </a:ln>
@@ -2693,44 +2611,108 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="dk1">
-          <a:lumMod val="50000"/>
-          <a:lumOff val="50000"/>
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
         </a:schemeClr>
       </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="75000"/>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
       </a:ln>
     </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="50000"/>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
       </a:ln>
     </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
@@ -2740,134 +2722,81 @@
     <cs:spPr>
       <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="50000"/>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
       </a:ln>
     </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-            <a:alpha val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-            <a:alpha val="25000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="50000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="50000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="75000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="75000"/>
-      </a:schemeClr>
-    </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:seriesAxis>
   <cs:seriesLine>
@@ -2880,8 +2809,9 @@
     <cs:spPr>
       <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="50000"/>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -2893,11 +2823,12 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="85000"/>
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="1400" b="1" kern="1200" cap="none" baseline="0"/>
+    <cs:defRPr sz="1600" b="1" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0"/>
   </cs:title>
   <cs:trendline>
     <cs:lnRef idx="0">
@@ -2906,14 +2837,12 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="25400" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:alpha val="50000"/>
-          </a:schemeClr>
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
         </a:solidFill>
       </a:ln>
     </cs:spPr>
@@ -2923,11 +2852,12 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="75000"/>
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
+    <cs:defRPr sz="800" kern="1200"/>
   </cs:trendlineLabel>
   <cs:upBar>
     <cs:lnRef idx="0"/>
@@ -2938,41 +2868,40 @@
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
-        <a:schemeClr val="lt1">
-          <a:lumMod val="85000"/>
-        </a:schemeClr>
+        <a:schemeClr val="lt1"/>
       </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
           <a:schemeClr val="dk1">
-            <a:lumMod val="50000"/>
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
       </a:ln>
     </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="75000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="50000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr/>
   </cs:valueAxis>
   <cs:wall>
     <cs:lnRef idx="0"/>
@@ -3340,8 +3269,8 @@
   </sheetPr>
   <dimension ref="A1:H24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="W18" sqref="W18"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="Y13" sqref="Y13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3356,438 +3285,438 @@
     <row r="1" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:8" ht="34.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2"/>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="5"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="4" t="s">
+      <c r="C2" s="15"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="5"/>
-      <c r="H2" s="6"/>
+      <c r="G2" s="15"/>
+      <c r="H2" s="16"/>
     </row>
     <row r="3" spans="1:8" ht="39" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="9" t="s">
+      <c r="D3" s="6" t="s">
         <v>1</v>
       </c>
       <c r="F3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="G3" s="8" t="s">
+      <c r="G3" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="H3" s="9" t="s">
+      <c r="H3" s="6" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="22.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="10">
+      <c r="B4" s="7">
         <v>10000</v>
       </c>
-      <c r="C4" s="11">
+      <c r="C4" s="8">
         <v>7.6116999999999999</v>
       </c>
-      <c r="D4" s="12">
+      <c r="D4" s="9">
         <v>16.957100000000001</v>
       </c>
-      <c r="F4" s="10">
+      <c r="F4" s="7">
         <v>10000</v>
       </c>
-      <c r="G4" s="11">
+      <c r="G4" s="8">
         <v>5.6723999999999997</v>
       </c>
-      <c r="H4" s="12">
+      <c r="H4" s="9">
         <v>26.4435</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="22.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="10">
+      <c r="B5" s="7">
         <v>20000</v>
       </c>
-      <c r="C5" s="11">
+      <c r="C5" s="8">
         <v>11.535299999999999</v>
       </c>
-      <c r="D5" s="12">
+      <c r="D5" s="9">
         <v>57.9893</v>
       </c>
-      <c r="F5" s="10">
+      <c r="F5" s="7">
         <v>20000</v>
       </c>
-      <c r="G5" s="11">
+      <c r="G5" s="8">
         <v>12.5158</v>
       </c>
-      <c r="H5" s="12">
+      <c r="H5" s="9">
         <v>100.952</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="22.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="10">
+      <c r="B6" s="7">
         <v>30000</v>
       </c>
-      <c r="C6" s="11">
+      <c r="C6" s="8">
         <v>18.3187</v>
       </c>
-      <c r="D6" s="12">
+      <c r="D6" s="9">
         <v>109.58</v>
       </c>
-      <c r="F6" s="10">
+      <c r="F6" s="7">
         <v>30000</v>
       </c>
-      <c r="G6" s="11">
+      <c r="G6" s="8">
         <v>18.057500000000001</v>
       </c>
-      <c r="H6" s="12">
+      <c r="H6" s="9">
         <v>264.06700000000001</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="22.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="10">
+      <c r="B7" s="7">
         <v>40000</v>
       </c>
-      <c r="C7" s="11">
+      <c r="C7" s="8">
         <v>23.6191</v>
       </c>
-      <c r="D7" s="12">
+      <c r="D7" s="9">
         <v>207.70099999999999</v>
       </c>
-      <c r="F7" s="10">
+      <c r="F7" s="7">
         <v>40000</v>
       </c>
-      <c r="G7" s="11">
+      <c r="G7" s="8">
         <v>20.020600000000002</v>
       </c>
-      <c r="H7" s="12">
+      <c r="H7" s="9">
         <v>452.726</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="22.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="10">
+      <c r="B8" s="7">
         <v>50000</v>
       </c>
-      <c r="C8" s="13">
+      <c r="C8" s="10">
         <v>26.335100000000001</v>
       </c>
-      <c r="D8" s="14">
+      <c r="D8" s="11">
         <v>444.07</v>
       </c>
-      <c r="E8" s="7"/>
-      <c r="F8" s="10">
+      <c r="E8" s="4"/>
+      <c r="F8" s="7">
         <v>50000</v>
       </c>
-      <c r="G8" s="13">
+      <c r="G8" s="10">
         <v>27.513500000000001</v>
       </c>
-      <c r="H8" s="14">
+      <c r="H8" s="11">
         <v>660.18399999999997</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="22.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="10">
+      <c r="B9" s="7">
         <v>60000</v>
       </c>
-      <c r="C9" s="13">
+      <c r="C9" s="10">
         <v>26.8992</v>
       </c>
-      <c r="D9" s="14">
+      <c r="D9" s="11">
         <v>662.39599999999996</v>
       </c>
-      <c r="E9" s="7"/>
-      <c r="F9" s="10">
+      <c r="E9" s="4"/>
+      <c r="F9" s="7">
         <v>60000</v>
       </c>
-      <c r="G9" s="13">
+      <c r="G9" s="10">
         <v>25.622399999999999</v>
       </c>
-      <c r="H9" s="14">
+      <c r="H9" s="11">
         <v>486.00200000000001</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="22.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="10">
+      <c r="B10" s="7">
         <v>70000</v>
       </c>
-      <c r="C10" s="13">
+      <c r="C10" s="10">
         <v>33.294199999999996</v>
       </c>
-      <c r="D10" s="14">
+      <c r="D10" s="11">
         <v>716.68499999999995</v>
       </c>
-      <c r="E10" s="7"/>
-      <c r="F10" s="10">
+      <c r="E10" s="4"/>
+      <c r="F10" s="7">
         <v>70000</v>
       </c>
-      <c r="G10" s="13">
+      <c r="G10" s="10">
         <v>36.346200000000003</v>
       </c>
-      <c r="H10" s="14">
+      <c r="H10" s="11">
         <v>885.423</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="22.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="10">
+      <c r="B11" s="7">
         <v>80000</v>
       </c>
-      <c r="C11" s="15">
+      <c r="C11" s="12">
         <v>42.598199999999999</v>
       </c>
-      <c r="D11" s="16">
+      <c r="D11" s="13">
         <v>883.04100000000005</v>
       </c>
-      <c r="F11" s="10">
+      <c r="F11" s="7">
         <v>80000</v>
       </c>
-      <c r="G11" s="15">
+      <c r="G11" s="12">
         <v>45.921100000000003</v>
       </c>
-      <c r="H11" s="16">
+      <c r="H11" s="13">
         <v>896.45699999999999</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="22.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="10">
+      <c r="B12" s="7">
         <v>90000</v>
       </c>
-      <c r="C12" s="15">
+      <c r="C12" s="12">
         <v>50.175600000000003</v>
       </c>
-      <c r="D12" s="16">
+      <c r="D12" s="13">
         <v>918.26400000000001</v>
       </c>
-      <c r="F12" s="10">
+      <c r="F12" s="7">
         <v>90000</v>
       </c>
-      <c r="G12" s="15">
+      <c r="G12" s="12">
         <v>50.270899999999997</v>
       </c>
-      <c r="H12" s="16">
+      <c r="H12" s="13">
         <v>914.36599999999999</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="22.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="10">
+      <c r="B13" s="7">
         <v>100000</v>
       </c>
-      <c r="C13" s="15">
+      <c r="C13" s="12">
         <v>56.835700000000003</v>
       </c>
-      <c r="D13" s="16">
+      <c r="D13" s="13">
         <v>937.01800000000003</v>
       </c>
-      <c r="F13" s="10">
+      <c r="F13" s="7">
         <v>100000</v>
       </c>
-      <c r="G13" s="15">
+      <c r="G13" s="12">
         <v>57.696300000000001</v>
       </c>
-      <c r="H13" s="16">
+      <c r="H13" s="13">
         <v>973.93600000000004</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="22.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="10">
+      <c r="B14" s="7">
         <v>110000</v>
       </c>
-      <c r="C14" s="15">
+      <c r="C14" s="12">
         <v>52.569299999999998</v>
       </c>
-      <c r="D14" s="16">
+      <c r="D14" s="13">
         <v>932.70899999999995</v>
       </c>
-      <c r="F14" s="10">
+      <c r="F14" s="7">
         <v>110000</v>
       </c>
-      <c r="G14" s="15">
+      <c r="G14" s="12">
         <v>51.777700000000003</v>
       </c>
-      <c r="H14" s="16">
+      <c r="H14" s="13">
         <v>525.30100000000004</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="22.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="10">
+      <c r="B15" s="7">
         <v>120000</v>
       </c>
-      <c r="C15" s="15">
+      <c r="C15" s="12">
         <v>57.937199999999997</v>
       </c>
-      <c r="D15" s="16">
+      <c r="D15" s="13">
         <v>955.053</v>
       </c>
-      <c r="F15" s="10">
+      <c r="F15" s="7">
         <v>120000</v>
       </c>
-      <c r="G15" s="15">
+      <c r="G15" s="12">
         <v>55.4998</v>
       </c>
-      <c r="H15" s="16">
+      <c r="H15" s="13">
         <v>559.07100000000003</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="22.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="10">
+      <c r="B16" s="7">
         <v>130000</v>
       </c>
-      <c r="C16" s="15">
+      <c r="C16" s="12">
         <v>64.104100000000003</v>
       </c>
-      <c r="D16" s="16">
+      <c r="D16" s="13">
         <v>1014.45</v>
       </c>
-      <c r="F16" s="10">
+      <c r="F16" s="7">
         <v>130000</v>
       </c>
-      <c r="G16" s="15">
+      <c r="G16" s="12">
         <v>66.572699999999998</v>
       </c>
-      <c r="H16" s="16">
+      <c r="H16" s="13">
         <v>610.85500000000002</v>
       </c>
     </row>
     <row r="17" spans="2:8" ht="22.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="10">
+      <c r="B17" s="7">
         <v>140000</v>
       </c>
-      <c r="C17" s="15">
+      <c r="C17" s="12">
         <v>63.8902</v>
       </c>
-      <c r="D17" s="16">
+      <c r="D17" s="13">
         <v>327.88600000000002</v>
       </c>
-      <c r="F17" s="10">
+      <c r="F17" s="7">
         <v>140000</v>
       </c>
-      <c r="G17" s="15">
+      <c r="G17" s="12">
         <v>68.846599999999995</v>
       </c>
-      <c r="H17" s="16">
+      <c r="H17" s="13">
         <v>327.952</v>
       </c>
     </row>
     <row r="18" spans="2:8" ht="22.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="10">
+      <c r="B18" s="7">
         <v>150000</v>
       </c>
-      <c r="C18" s="15">
+      <c r="C18" s="12">
         <v>72.808199999999999</v>
       </c>
-      <c r="D18" s="16">
+      <c r="D18" s="13">
         <v>327.26100000000002</v>
       </c>
-      <c r="F18" s="10">
+      <c r="F18" s="7">
         <v>150000</v>
       </c>
-      <c r="G18" s="15">
+      <c r="G18" s="12">
         <v>79.3185</v>
       </c>
-      <c r="H18" s="16">
+      <c r="H18" s="13">
         <v>334.78699999999998</v>
       </c>
     </row>
     <row r="19" spans="2:8" ht="22.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="10">
+      <c r="B19" s="7">
         <v>160000</v>
       </c>
-      <c r="C19" s="15">
+      <c r="C19" s="12">
         <v>79.025499999999994</v>
       </c>
-      <c r="D19" s="16">
+      <c r="D19" s="13">
         <v>343.11500000000001</v>
       </c>
-      <c r="F19" s="10">
+      <c r="F19" s="7">
         <v>160000</v>
       </c>
-      <c r="G19" s="15">
+      <c r="G19" s="12">
         <v>83.187399999999997</v>
       </c>
-      <c r="H19" s="16">
+      <c r="H19" s="13">
         <v>348.49299999999999</v>
       </c>
     </row>
     <row r="20" spans="2:8" ht="22.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="10">
+      <c r="B20" s="7">
         <v>170000</v>
       </c>
-      <c r="C20" s="15">
+      <c r="C20" s="12">
         <v>85.820099999999996</v>
       </c>
-      <c r="D20" s="16">
+      <c r="D20" s="13">
         <v>350.041</v>
       </c>
-      <c r="F20" s="10">
+      <c r="F20" s="7">
         <v>170000</v>
       </c>
-      <c r="G20" s="15">
+      <c r="G20" s="12">
         <v>91.867999999999995</v>
       </c>
-      <c r="H20" s="16">
+      <c r="H20" s="13">
         <v>349.81200000000001</v>
       </c>
     </row>
     <row r="21" spans="2:8" ht="22.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="10">
+      <c r="B21" s="7">
         <v>180000</v>
       </c>
-      <c r="C21" s="15">
+      <c r="C21" s="12">
         <v>92.818399999999997</v>
       </c>
-      <c r="D21" s="16">
+      <c r="D21" s="13">
         <v>361.14400000000001</v>
       </c>
-      <c r="F21" s="10">
+      <c r="F21" s="7">
         <v>180000</v>
       </c>
-      <c r="G21" s="15">
+      <c r="G21" s="12">
         <v>97.1935</v>
       </c>
-      <c r="H21" s="16">
+      <c r="H21" s="13">
         <v>360.58800000000002</v>
       </c>
     </row>
     <row r="22" spans="2:8" ht="22.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="10">
+      <c r="B22" s="7">
         <v>190000</v>
       </c>
-      <c r="C22" s="15">
+      <c r="C22" s="12">
         <v>100.321</v>
       </c>
-      <c r="D22" s="16">
+      <c r="D22" s="13">
         <v>368.10199999999998</v>
       </c>
-      <c r="F22" s="10">
+      <c r="F22" s="7">
         <v>190000</v>
       </c>
-      <c r="G22" s="15">
+      <c r="G22" s="12">
         <v>103.254</v>
       </c>
-      <c r="H22" s="16">
+      <c r="H22" s="13">
         <v>375.02300000000002</v>
       </c>
     </row>
     <row r="23" spans="2:8" ht="22.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="10">
+      <c r="B23" s="7">
         <v>200000</v>
       </c>
-      <c r="C23" s="15">
+      <c r="C23" s="12">
         <v>108.145</v>
       </c>
-      <c r="D23" s="16">
+      <c r="D23" s="13">
         <v>384.428</v>
       </c>
-      <c r="F23" s="10">
+      <c r="F23" s="7">
         <v>200000</v>
       </c>
-      <c r="G23" s="15">
+      <c r="G23" s="12">
         <v>112.639</v>
       </c>
-      <c r="H23" s="16">
+      <c r="H23" s="13">
         <v>390.89</v>
       </c>
     </row>

</xml_diff>